<commit_message>
update DB schema @Author : Alex
</commit_message>
<xml_diff>
--- a/05 Q&A/问答一览表.xlsx
+++ b/05 Q&A/问答一览表.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="118">
   <si>
     <t>版本履历</t>
   </si>
@@ -321,6 +321,97 @@
 </t>
   </si>
   <si>
+    <t>中兴的接口好像不稳定，有时会出现如下错误
+org.springframework.web.client.ResourceAccessException: I/O error on GET request for "http://client.wostore.cn:6106/appstore_agent/unistore/servicedata.do?serviceid=productdetail&amp;productid=187834&amp;state=101":Server redirected too many  times (20); nested exception is java.net.ProtocolException: Server redirected too many  times (20)</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>建议到联通驻场开发，如有问题立刻联系</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>多渠道下载问题
+1.中兴侧如果不支持“_”，则可能会在篡改下载URL是去掉“_”。
+2.31省渠道包和沃游戏，沃商店的渠道包同时存在，但沃商店的渠道包是最新的包的时候。下载哪个渠道包</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.等联调结果，做判定
+2.下载最新的沃商店的渠道包</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>沈鹏
+黄国腾</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>殷专成</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载问题
+中兴沃商店下载接口中，header头中的clientchannelflag的意义</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>为8时，表示从沃游戏过来的下载。中兴侧先下载沃游戏的渠道包，没有则下载沃商店的渠道包
+为空时（不填），直接下载沃商店的渠道包
+沃游戏中心，直接获取沃商店的下载URL，然后判断是否篡改URL</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>路翠萍</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEV部署环境</t>
+  </si>
+  <si>
+    <t>14/06/26</t>
+  </si>
+  <si>
+    <t>阮涛
+石少飞</t>
+  </si>
+  <si>
+    <t>搜索初始页面显示列表内容（参照沃游戏）</t>
+  </si>
+  <si>
+    <t>Q016</t>
+  </si>
+  <si>
+    <t>Q017</t>
+  </si>
+  <si>
+    <t>Q018</t>
+  </si>
+  <si>
+    <t>沃游戏APP的推荐页，两栏的游戏只显示第一条游戏。
+WAP端的如何显示？</t>
+  </si>
+  <si>
+    <t>ad_type: 4,                     
+# 推荐位类型 1：单栏 2：双栏 4：四栏
+我测试了一下，其adType为1。我们只需显示一条游戏</t>
+  </si>
+  <si>
+    <t>热词：
+联想词：2.46 获取热门关键字列表getkeywords</t>
+  </si>
+  <si>
+    <t>两栏游戏应该显示2个的。广告位是可以选择的，单栏、双栏、4栏，目前是这3种。比如运营操作第一次选择了4栏广告位，添加了4个游戏，之后又将这个4栏广告位改成了2栏广告位，那么原来添加的4个游戏2个做了修改需要显示，另外两个就是不需要显示的数据。所以做了处理只显示前2个。
+该游戏为单栏游戏，只需显示一条</t>
+  </si>
+  <si>
     <t>这个是每个游戏的角标。
 &lt;option value="0"&gt;普通推荐&lt;/option&gt; 
  &lt;option value="1"&gt;最新发布&lt;/option&gt; 
@@ -335,30 +426,10 @@
  &lt;option value="10" selected="selected"&gt;新星&lt;/option&gt; 
  &lt;option value="11"&gt;奇葩&lt;/option&gt;
 0普通推荐不要处理</t>
-  </si>
-  <si>
-    <t>中兴的接口好像不稳定，有时会出现如下错误
-org.springframework.web.client.ResourceAccessException: I/O error on GET request for "http://client.wostore.cn:6106/appstore_agent/unistore/servicedata.do?serviceid=productdetail&amp;productid=187834&amp;state=101":Server redirected too many  times (20); nested exception is java.net.ProtocolException: Server redirected too many  times (20)</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
-    <t>建议到联通驻场开发，如有问题立刻联系</t>
-    <phoneticPr fontId="37" type="noConversion"/>
-  </si>
-  <si>
-    <t>多渠道下载问题
-1.中兴侧如果不支持“_”，则可能会在篡改下载URL是去掉“_”。
-2.31省渠道包和沃游戏，沃商店的渠道包同时存在，但沃商店的渠道包是最新的包的时候。下载哪个渠道包</t>
-    <phoneticPr fontId="37" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.等联调结果，做判定
-2.下载最新的沃商店的渠道包</t>
-    <phoneticPr fontId="37" type="noConversion"/>
-  </si>
-  <si>
-    <t>沈鹏
-黄国腾</t>
+    <t>目前分类中有个 ［最热下载］的角标，但是上次说的[Q008]角标中没有包含</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
@@ -366,18 +437,12 @@
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
-    <t>下载问题
-中兴沃商店下载接口中，header头中的clientchannelflag的意义</t>
+    <t>殷专成</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
-    <t>为8时，表示从沃游戏过来的下载。中兴侧先下载沃游戏的渠道包，没有则下载沃商店的渠道包
-为空时（不填），直接下载沃商店的渠道包
-沃游戏中心，直接获取沃商店的下载URL，然后判断是否篡改URL</t>
-    <phoneticPr fontId="37" type="noConversion"/>
-  </si>
-  <si>
-    <t>路翠萍</t>
+    <t>【最热下载】其实为【最热发布】（value=2）
+这两个是一样的~可能之前他们整理的时候打错字了~</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
@@ -385,68 +450,55 @@
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
-    <t>设计</t>
+    <t>顾蕾</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
-    <t>DEV部署环境</t>
-  </si>
-  <si>
-    <t>14/06/26</t>
-  </si>
-  <si>
-    <t>阮涛
-石少飞</t>
-  </si>
-  <si>
-    <t>搜索初始页面显示列表内容（参照沃游戏）</t>
-  </si>
-  <si>
-    <t>Q016</t>
-  </si>
-  <si>
-    <t>Q017</t>
-  </si>
-  <si>
-    <t>Q018</t>
-  </si>
-  <si>
-    <t>沃游戏APP的推荐页，两栏的游戏只显示第一条游戏。
-WAP端的如何显示？</t>
-  </si>
-  <si>
-    <t>ad_type: 4,                     
-# 推荐位类型 1：单栏 2：双栏 4：四栏
-我测试了一下，其adType为1。我们只需显示一条游戏</t>
-  </si>
-  <si>
-    <t>热词：
-联想词：2.46 获取热门关键字列表getkeywords</t>
+    <t>123.125.219.83
+用户名：root 
+密码：wyyx!@#$
+开发测试环境 
+linux 系统  全新的 啥都没有 需要自己安装</t>
+    <phoneticPr fontId="37" type="noConversion"/>
   </si>
   <si>
     <t>搜索页面下面的热词
-（是联通后台自己维护的，运营可以自己添加。应该有个接口的。顾蕾明天会帮忙问搜索人员。）
+（是联通后台自己维护的，运营可以自己添加。接口：http://wogame.wostore.cn:8080/gameservice/hotwordsList.do。）
 输入文字的时候出现的联想词
 （调用中兴接口）</t>
-  </si>
-  <si>
-    <t>两栏游戏应该显示2个的。广告位是可以选择的，单栏、双栏、4栏，目前是这3种。比如运营操作第一次选择了4栏广告位，添加了4个游戏，之后又将这个4栏广告位改成了2栏广告位，那么原来添加的4个游戏2个做了修改需要显示，另外两个就是不需要显示的数据。所以做了处理只显示前2个。
-该游戏为单栏游戏，只需显示一条</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>回执文件</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>210.22.123.95:21
+package/p3temp_S</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>朱自明</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发</t>
+    <phoneticPr fontId="37" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
-    <numFmt numFmtId="165" formatCode="yy/mm/dd"/>
+    <numFmt numFmtId="176" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
+    <numFmt numFmtId="177" formatCode="yy/mm/dd"/>
   </numFmts>
   <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -701,7 +753,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1142,7 +1194,7 @@
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1261,7 +1313,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="12" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="12" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1326,10 +1378,10 @@
     <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="27" borderId="12" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="32" fillId="27" borderId="12" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="12" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="12" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1338,20 +1390,20 @@
     <xf numFmtId="0" fontId="32" fillId="26" borderId="19" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="57">
@@ -1376,9 +1428,7 @@
     <cellStyle name="Calc Currency (0)" xfId="20"/>
     <cellStyle name="Header1" xfId="21"/>
     <cellStyle name="Header2" xfId="22"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8"/>
     <cellStyle name="JIKK040E" xfId="23"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="56"/>
     <cellStyle name="qqq" xfId="24"/>
@@ -1394,96 +1444,28 @@
     <cellStyle name="どちらでもない" xfId="34"/>
     <cellStyle name="メモ" xfId="35"/>
     <cellStyle name="リンク セル" xfId="36"/>
-    <cellStyle name="入力" xfId="37"/>
+    <cellStyle name="標準_ＤＲ報告書（ＴＧ前レビュー）" xfId="45"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8"/>
     <cellStyle name="出力" xfId="38"/>
-    <cellStyle name="原価計算" xfId="39"/>
+    <cellStyle name="悪い" xfId="43"/>
+    <cellStyle name="工数集計" xfId="42"/>
     <cellStyle name="基本計画検討書（PJ）" xfId="40"/>
     <cellStyle name="基本計画検討書（通番）" xfId="41"/>
-    <cellStyle name="工数集計" xfId="42"/>
-    <cellStyle name="悪い" xfId="43"/>
-    <cellStyle name="未定義" xfId="44"/>
-    <cellStyle name="標準_ＤＲ報告書（ＴＧ前レビュー）" xfId="45"/>
-    <cellStyle name="良い" xfId="46"/>
+    <cellStyle name="集計" xfId="54"/>
+    <cellStyle name="計算" xfId="51"/>
     <cellStyle name="見出し 1" xfId="47"/>
     <cellStyle name="見出し 2" xfId="48"/>
     <cellStyle name="見出し 3" xfId="49"/>
     <cellStyle name="見出し 4" xfId="50"/>
-    <cellStyle name="計算" xfId="51"/>
+    <cellStyle name="警告文" xfId="53"/>
+    <cellStyle name="良い" xfId="46"/>
+    <cellStyle name="入力" xfId="37"/>
     <cellStyle name="説明文" xfId="52"/>
-    <cellStyle name="警告文" xfId="53"/>
-    <cellStyle name="集計" xfId="54"/>
+    <cellStyle name="未定義" xfId="44"/>
+    <cellStyle name="原価計算" xfId="39"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="53"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="53"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="53"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="53"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="53"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -1594,7 +1576,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="版本履历"/>
@@ -1705,7 +1687,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1779,6 +1761,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1813,6 +1796,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1988,23 +1972,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" style="33" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="33" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="33" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="33" customWidth="1"/>
-    <col min="5" max="9" width="9.140625" style="33" customWidth="1"/>
-    <col min="10" max="10" width="1.85546875" style="33" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="33" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="33"/>
+    <col min="1" max="1" width="1.875" style="33" customWidth="1"/>
+    <col min="2" max="2" width="6.875" style="33" customWidth="1"/>
+    <col min="3" max="3" width="9.125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="33" customWidth="1"/>
+    <col min="5" max="9" width="9.125" style="33" customWidth="1"/>
+    <col min="10" max="10" width="1.875" style="33" customWidth="1"/>
+    <col min="11" max="12" width="9.125" style="33" customWidth="1"/>
+    <col min="13" max="16384" width="9.125" style="33"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" s="26" customFormat="1" ht="19.5" customHeight="1">
@@ -2313,6 +2297,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F8:I8"/>
@@ -2325,15 +2318,6 @@
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
   </mergeCells>
   <phoneticPr fontId="37" type="noConversion"/>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.31458333333333299" footer="0.31458333333333299"/>
@@ -2346,1045 +2330,1045 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="4" topLeftCell="N14" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="11" ySplit="4" topLeftCell="L17" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q38" sqref="Q38"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="6.375" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="2" style="4" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="7.625" style="4" customWidth="1"/>
     <col min="3" max="7" width="9" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="10.25" style="11" customWidth="1"/>
+    <col min="9" max="9" width="12.75" style="11" customWidth="1"/>
     <col min="10" max="11" width="9" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="11" customWidth="1"/>
-    <col min="13" max="15" width="10.28515625" style="11" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="6.7109375" style="11" customWidth="1"/>
-    <col min="17" max="18" width="10.28515625" style="11" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="10.42578125" style="4" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="10.25" style="11" customWidth="1"/>
+    <col min="13" max="15" width="10.25" style="11" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="6.75" style="11" customWidth="1"/>
+    <col min="17" max="18" width="10.25" style="11" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="10.375" style="4" customWidth="1" outlineLevel="1"/>
     <col min="20" max="23" width="9" style="4" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="10.28515625" style="11" customWidth="1"/>
-    <col min="25" max="26" width="8.28515625" style="11" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="31" width="6.42578125" style="4" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="256" width="6.42578125" style="4"/>
+    <col min="24" max="24" width="10.25" style="11" customWidth="1"/>
+    <col min="25" max="26" width="8.25" style="11" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="31" width="6.375" style="4" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="256" width="6.375" style="4"/>
     <col min="257" max="257" width="2" style="4" customWidth="1"/>
-    <col min="258" max="258" width="7.5703125" style="4" customWidth="1"/>
+    <col min="258" max="258" width="7.625" style="4" customWidth="1"/>
     <col min="259" max="263" width="9" style="4" customWidth="1"/>
-    <col min="264" max="264" width="10.28515625" style="4" customWidth="1"/>
-    <col min="265" max="265" width="12.7109375" style="4" customWidth="1"/>
+    <col min="264" max="264" width="10.25" style="4" customWidth="1"/>
+    <col min="265" max="265" width="12.75" style="4" customWidth="1"/>
     <col min="266" max="266" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="267" max="267" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="268" max="271" width="10.28515625" style="4" customWidth="1"/>
-    <col min="272" max="272" width="6.7109375" style="4" customWidth="1"/>
-    <col min="273" max="274" width="10.28515625" style="4" customWidth="1"/>
-    <col min="275" max="275" width="10.42578125" style="4" customWidth="1"/>
+    <col min="268" max="271" width="10.25" style="4" customWidth="1"/>
+    <col min="272" max="272" width="6.75" style="4" customWidth="1"/>
+    <col min="273" max="274" width="10.25" style="4" customWidth="1"/>
+    <col min="275" max="275" width="10.375" style="4" customWidth="1"/>
     <col min="276" max="279" width="9" style="4" customWidth="1"/>
-    <col min="280" max="280" width="10.28515625" style="4" customWidth="1"/>
-    <col min="281" max="282" width="8.28515625" style="4" customWidth="1"/>
-    <col min="283" max="287" width="6.42578125" style="4" customWidth="1"/>
-    <col min="288" max="512" width="6.42578125" style="4"/>
+    <col min="280" max="280" width="10.25" style="4" customWidth="1"/>
+    <col min="281" max="282" width="8.25" style="4" customWidth="1"/>
+    <col min="283" max="287" width="6.375" style="4" customWidth="1"/>
+    <col min="288" max="512" width="6.375" style="4"/>
     <col min="513" max="513" width="2" style="4" customWidth="1"/>
-    <col min="514" max="514" width="7.5703125" style="4" customWidth="1"/>
+    <col min="514" max="514" width="7.625" style="4" customWidth="1"/>
     <col min="515" max="519" width="9" style="4" customWidth="1"/>
-    <col min="520" max="520" width="10.28515625" style="4" customWidth="1"/>
-    <col min="521" max="521" width="12.7109375" style="4" customWidth="1"/>
+    <col min="520" max="520" width="10.25" style="4" customWidth="1"/>
+    <col min="521" max="521" width="12.75" style="4" customWidth="1"/>
     <col min="522" max="522" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="523" max="523" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="524" max="527" width="10.28515625" style="4" customWidth="1"/>
-    <col min="528" max="528" width="6.7109375" style="4" customWidth="1"/>
-    <col min="529" max="530" width="10.28515625" style="4" customWidth="1"/>
-    <col min="531" max="531" width="10.42578125" style="4" customWidth="1"/>
+    <col min="524" max="527" width="10.25" style="4" customWidth="1"/>
+    <col min="528" max="528" width="6.75" style="4" customWidth="1"/>
+    <col min="529" max="530" width="10.25" style="4" customWidth="1"/>
+    <col min="531" max="531" width="10.375" style="4" customWidth="1"/>
     <col min="532" max="535" width="9" style="4" customWidth="1"/>
-    <col min="536" max="536" width="10.28515625" style="4" customWidth="1"/>
-    <col min="537" max="538" width="8.28515625" style="4" customWidth="1"/>
-    <col min="539" max="543" width="6.42578125" style="4" customWidth="1"/>
-    <col min="544" max="768" width="6.42578125" style="4"/>
+    <col min="536" max="536" width="10.25" style="4" customWidth="1"/>
+    <col min="537" max="538" width="8.25" style="4" customWidth="1"/>
+    <col min="539" max="543" width="6.375" style="4" customWidth="1"/>
+    <col min="544" max="768" width="6.375" style="4"/>
     <col min="769" max="769" width="2" style="4" customWidth="1"/>
-    <col min="770" max="770" width="7.5703125" style="4" customWidth="1"/>
+    <col min="770" max="770" width="7.625" style="4" customWidth="1"/>
     <col min="771" max="775" width="9" style="4" customWidth="1"/>
-    <col min="776" max="776" width="10.28515625" style="4" customWidth="1"/>
-    <col min="777" max="777" width="12.7109375" style="4" customWidth="1"/>
+    <col min="776" max="776" width="10.25" style="4" customWidth="1"/>
+    <col min="777" max="777" width="12.75" style="4" customWidth="1"/>
     <col min="778" max="778" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="779" max="779" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="780" max="783" width="10.28515625" style="4" customWidth="1"/>
-    <col min="784" max="784" width="6.7109375" style="4" customWidth="1"/>
-    <col min="785" max="786" width="10.28515625" style="4" customWidth="1"/>
-    <col min="787" max="787" width="10.42578125" style="4" customWidth="1"/>
+    <col min="780" max="783" width="10.25" style="4" customWidth="1"/>
+    <col min="784" max="784" width="6.75" style="4" customWidth="1"/>
+    <col min="785" max="786" width="10.25" style="4" customWidth="1"/>
+    <col min="787" max="787" width="10.375" style="4" customWidth="1"/>
     <col min="788" max="791" width="9" style="4" customWidth="1"/>
-    <col min="792" max="792" width="10.28515625" style="4" customWidth="1"/>
-    <col min="793" max="794" width="8.28515625" style="4" customWidth="1"/>
-    <col min="795" max="799" width="6.42578125" style="4" customWidth="1"/>
-    <col min="800" max="1024" width="6.42578125" style="4"/>
+    <col min="792" max="792" width="10.25" style="4" customWidth="1"/>
+    <col min="793" max="794" width="8.25" style="4" customWidth="1"/>
+    <col min="795" max="799" width="6.375" style="4" customWidth="1"/>
+    <col min="800" max="1024" width="6.375" style="4"/>
     <col min="1025" max="1025" width="2" style="4" customWidth="1"/>
-    <col min="1026" max="1026" width="7.5703125" style="4" customWidth="1"/>
+    <col min="1026" max="1026" width="7.625" style="4" customWidth="1"/>
     <col min="1027" max="1031" width="9" style="4" customWidth="1"/>
-    <col min="1032" max="1032" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1033" max="1033" width="12.7109375" style="4" customWidth="1"/>
+    <col min="1032" max="1032" width="10.25" style="4" customWidth="1"/>
+    <col min="1033" max="1033" width="12.75" style="4" customWidth="1"/>
     <col min="1034" max="1034" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="1035" max="1035" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="1036" max="1039" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1040" max="1040" width="6.7109375" style="4" customWidth="1"/>
-    <col min="1041" max="1042" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1043" max="1043" width="10.42578125" style="4" customWidth="1"/>
+    <col min="1036" max="1039" width="10.25" style="4" customWidth="1"/>
+    <col min="1040" max="1040" width="6.75" style="4" customWidth="1"/>
+    <col min="1041" max="1042" width="10.25" style="4" customWidth="1"/>
+    <col min="1043" max="1043" width="10.375" style="4" customWidth="1"/>
     <col min="1044" max="1047" width="9" style="4" customWidth="1"/>
-    <col min="1048" max="1048" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1049" max="1050" width="8.28515625" style="4" customWidth="1"/>
-    <col min="1051" max="1055" width="6.42578125" style="4" customWidth="1"/>
-    <col min="1056" max="1280" width="6.42578125" style="4"/>
+    <col min="1048" max="1048" width="10.25" style="4" customWidth="1"/>
+    <col min="1049" max="1050" width="8.25" style="4" customWidth="1"/>
+    <col min="1051" max="1055" width="6.375" style="4" customWidth="1"/>
+    <col min="1056" max="1280" width="6.375" style="4"/>
     <col min="1281" max="1281" width="2" style="4" customWidth="1"/>
-    <col min="1282" max="1282" width="7.5703125" style="4" customWidth="1"/>
+    <col min="1282" max="1282" width="7.625" style="4" customWidth="1"/>
     <col min="1283" max="1287" width="9" style="4" customWidth="1"/>
-    <col min="1288" max="1288" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1289" max="1289" width="12.7109375" style="4" customWidth="1"/>
+    <col min="1288" max="1288" width="10.25" style="4" customWidth="1"/>
+    <col min="1289" max="1289" width="12.75" style="4" customWidth="1"/>
     <col min="1290" max="1290" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="1291" max="1291" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="1292" max="1295" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1296" max="1296" width="6.7109375" style="4" customWidth="1"/>
-    <col min="1297" max="1298" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1299" max="1299" width="10.42578125" style="4" customWidth="1"/>
+    <col min="1292" max="1295" width="10.25" style="4" customWidth="1"/>
+    <col min="1296" max="1296" width="6.75" style="4" customWidth="1"/>
+    <col min="1297" max="1298" width="10.25" style="4" customWidth="1"/>
+    <col min="1299" max="1299" width="10.375" style="4" customWidth="1"/>
     <col min="1300" max="1303" width="9" style="4" customWidth="1"/>
-    <col min="1304" max="1304" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1305" max="1306" width="8.28515625" style="4" customWidth="1"/>
-    <col min="1307" max="1311" width="6.42578125" style="4" customWidth="1"/>
-    <col min="1312" max="1536" width="6.42578125" style="4"/>
+    <col min="1304" max="1304" width="10.25" style="4" customWidth="1"/>
+    <col min="1305" max="1306" width="8.25" style="4" customWidth="1"/>
+    <col min="1307" max="1311" width="6.375" style="4" customWidth="1"/>
+    <col min="1312" max="1536" width="6.375" style="4"/>
     <col min="1537" max="1537" width="2" style="4" customWidth="1"/>
-    <col min="1538" max="1538" width="7.5703125" style="4" customWidth="1"/>
+    <col min="1538" max="1538" width="7.625" style="4" customWidth="1"/>
     <col min="1539" max="1543" width="9" style="4" customWidth="1"/>
-    <col min="1544" max="1544" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1545" max="1545" width="12.7109375" style="4" customWidth="1"/>
+    <col min="1544" max="1544" width="10.25" style="4" customWidth="1"/>
+    <col min="1545" max="1545" width="12.75" style="4" customWidth="1"/>
     <col min="1546" max="1546" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="1547" max="1547" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="1548" max="1551" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1552" max="1552" width="6.7109375" style="4" customWidth="1"/>
-    <col min="1553" max="1554" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1555" max="1555" width="10.42578125" style="4" customWidth="1"/>
+    <col min="1548" max="1551" width="10.25" style="4" customWidth="1"/>
+    <col min="1552" max="1552" width="6.75" style="4" customWidth="1"/>
+    <col min="1553" max="1554" width="10.25" style="4" customWidth="1"/>
+    <col min="1555" max="1555" width="10.375" style="4" customWidth="1"/>
     <col min="1556" max="1559" width="9" style="4" customWidth="1"/>
-    <col min="1560" max="1560" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1561" max="1562" width="8.28515625" style="4" customWidth="1"/>
-    <col min="1563" max="1567" width="6.42578125" style="4" customWidth="1"/>
-    <col min="1568" max="1792" width="6.42578125" style="4"/>
+    <col min="1560" max="1560" width="10.25" style="4" customWidth="1"/>
+    <col min="1561" max="1562" width="8.25" style="4" customWidth="1"/>
+    <col min="1563" max="1567" width="6.375" style="4" customWidth="1"/>
+    <col min="1568" max="1792" width="6.375" style="4"/>
     <col min="1793" max="1793" width="2" style="4" customWidth="1"/>
-    <col min="1794" max="1794" width="7.5703125" style="4" customWidth="1"/>
+    <col min="1794" max="1794" width="7.625" style="4" customWidth="1"/>
     <col min="1795" max="1799" width="9" style="4" customWidth="1"/>
-    <col min="1800" max="1800" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1801" max="1801" width="12.7109375" style="4" customWidth="1"/>
+    <col min="1800" max="1800" width="10.25" style="4" customWidth="1"/>
+    <col min="1801" max="1801" width="12.75" style="4" customWidth="1"/>
     <col min="1802" max="1802" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="1803" max="1803" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="1804" max="1807" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1808" max="1808" width="6.7109375" style="4" customWidth="1"/>
-    <col min="1809" max="1810" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1811" max="1811" width="10.42578125" style="4" customWidth="1"/>
+    <col min="1804" max="1807" width="10.25" style="4" customWidth="1"/>
+    <col min="1808" max="1808" width="6.75" style="4" customWidth="1"/>
+    <col min="1809" max="1810" width="10.25" style="4" customWidth="1"/>
+    <col min="1811" max="1811" width="10.375" style="4" customWidth="1"/>
     <col min="1812" max="1815" width="9" style="4" customWidth="1"/>
-    <col min="1816" max="1816" width="10.28515625" style="4" customWidth="1"/>
-    <col min="1817" max="1818" width="8.28515625" style="4" customWidth="1"/>
-    <col min="1819" max="1823" width="6.42578125" style="4" customWidth="1"/>
-    <col min="1824" max="2048" width="6.42578125" style="4"/>
+    <col min="1816" max="1816" width="10.25" style="4" customWidth="1"/>
+    <col min="1817" max="1818" width="8.25" style="4" customWidth="1"/>
+    <col min="1819" max="1823" width="6.375" style="4" customWidth="1"/>
+    <col min="1824" max="2048" width="6.375" style="4"/>
     <col min="2049" max="2049" width="2" style="4" customWidth="1"/>
-    <col min="2050" max="2050" width="7.5703125" style="4" customWidth="1"/>
+    <col min="2050" max="2050" width="7.625" style="4" customWidth="1"/>
     <col min="2051" max="2055" width="9" style="4" customWidth="1"/>
-    <col min="2056" max="2056" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2057" max="2057" width="12.7109375" style="4" customWidth="1"/>
+    <col min="2056" max="2056" width="10.25" style="4" customWidth="1"/>
+    <col min="2057" max="2057" width="12.75" style="4" customWidth="1"/>
     <col min="2058" max="2058" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="2059" max="2059" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="2060" max="2063" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2064" max="2064" width="6.7109375" style="4" customWidth="1"/>
-    <col min="2065" max="2066" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2067" max="2067" width="10.42578125" style="4" customWidth="1"/>
+    <col min="2060" max="2063" width="10.25" style="4" customWidth="1"/>
+    <col min="2064" max="2064" width="6.75" style="4" customWidth="1"/>
+    <col min="2065" max="2066" width="10.25" style="4" customWidth="1"/>
+    <col min="2067" max="2067" width="10.375" style="4" customWidth="1"/>
     <col min="2068" max="2071" width="9" style="4" customWidth="1"/>
-    <col min="2072" max="2072" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2073" max="2074" width="8.28515625" style="4" customWidth="1"/>
-    <col min="2075" max="2079" width="6.42578125" style="4" customWidth="1"/>
-    <col min="2080" max="2304" width="6.42578125" style="4"/>
+    <col min="2072" max="2072" width="10.25" style="4" customWidth="1"/>
+    <col min="2073" max="2074" width="8.25" style="4" customWidth="1"/>
+    <col min="2075" max="2079" width="6.375" style="4" customWidth="1"/>
+    <col min="2080" max="2304" width="6.375" style="4"/>
     <col min="2305" max="2305" width="2" style="4" customWidth="1"/>
-    <col min="2306" max="2306" width="7.5703125" style="4" customWidth="1"/>
+    <col min="2306" max="2306" width="7.625" style="4" customWidth="1"/>
     <col min="2307" max="2311" width="9" style="4" customWidth="1"/>
-    <col min="2312" max="2312" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2313" max="2313" width="12.7109375" style="4" customWidth="1"/>
+    <col min="2312" max="2312" width="10.25" style="4" customWidth="1"/>
+    <col min="2313" max="2313" width="12.75" style="4" customWidth="1"/>
     <col min="2314" max="2314" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="2315" max="2315" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="2316" max="2319" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2320" max="2320" width="6.7109375" style="4" customWidth="1"/>
-    <col min="2321" max="2322" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2323" max="2323" width="10.42578125" style="4" customWidth="1"/>
+    <col min="2316" max="2319" width="10.25" style="4" customWidth="1"/>
+    <col min="2320" max="2320" width="6.75" style="4" customWidth="1"/>
+    <col min="2321" max="2322" width="10.25" style="4" customWidth="1"/>
+    <col min="2323" max="2323" width="10.375" style="4" customWidth="1"/>
     <col min="2324" max="2327" width="9" style="4" customWidth="1"/>
-    <col min="2328" max="2328" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2329" max="2330" width="8.28515625" style="4" customWidth="1"/>
-    <col min="2331" max="2335" width="6.42578125" style="4" customWidth="1"/>
-    <col min="2336" max="2560" width="6.42578125" style="4"/>
+    <col min="2328" max="2328" width="10.25" style="4" customWidth="1"/>
+    <col min="2329" max="2330" width="8.25" style="4" customWidth="1"/>
+    <col min="2331" max="2335" width="6.375" style="4" customWidth="1"/>
+    <col min="2336" max="2560" width="6.375" style="4"/>
     <col min="2561" max="2561" width="2" style="4" customWidth="1"/>
-    <col min="2562" max="2562" width="7.5703125" style="4" customWidth="1"/>
+    <col min="2562" max="2562" width="7.625" style="4" customWidth="1"/>
     <col min="2563" max="2567" width="9" style="4" customWidth="1"/>
-    <col min="2568" max="2568" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2569" max="2569" width="12.7109375" style="4" customWidth="1"/>
+    <col min="2568" max="2568" width="10.25" style="4" customWidth="1"/>
+    <col min="2569" max="2569" width="12.75" style="4" customWidth="1"/>
     <col min="2570" max="2570" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="2571" max="2571" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="2572" max="2575" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2576" max="2576" width="6.7109375" style="4" customWidth="1"/>
-    <col min="2577" max="2578" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2579" max="2579" width="10.42578125" style="4" customWidth="1"/>
+    <col min="2572" max="2575" width="10.25" style="4" customWidth="1"/>
+    <col min="2576" max="2576" width="6.75" style="4" customWidth="1"/>
+    <col min="2577" max="2578" width="10.25" style="4" customWidth="1"/>
+    <col min="2579" max="2579" width="10.375" style="4" customWidth="1"/>
     <col min="2580" max="2583" width="9" style="4" customWidth="1"/>
-    <col min="2584" max="2584" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2585" max="2586" width="8.28515625" style="4" customWidth="1"/>
-    <col min="2587" max="2591" width="6.42578125" style="4" customWidth="1"/>
-    <col min="2592" max="2816" width="6.42578125" style="4"/>
+    <col min="2584" max="2584" width="10.25" style="4" customWidth="1"/>
+    <col min="2585" max="2586" width="8.25" style="4" customWidth="1"/>
+    <col min="2587" max="2591" width="6.375" style="4" customWidth="1"/>
+    <col min="2592" max="2816" width="6.375" style="4"/>
     <col min="2817" max="2817" width="2" style="4" customWidth="1"/>
-    <col min="2818" max="2818" width="7.5703125" style="4" customWidth="1"/>
+    <col min="2818" max="2818" width="7.625" style="4" customWidth="1"/>
     <col min="2819" max="2823" width="9" style="4" customWidth="1"/>
-    <col min="2824" max="2824" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2825" max="2825" width="12.7109375" style="4" customWidth="1"/>
+    <col min="2824" max="2824" width="10.25" style="4" customWidth="1"/>
+    <col min="2825" max="2825" width="12.75" style="4" customWidth="1"/>
     <col min="2826" max="2826" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="2827" max="2827" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="2828" max="2831" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2832" max="2832" width="6.7109375" style="4" customWidth="1"/>
-    <col min="2833" max="2834" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2835" max="2835" width="10.42578125" style="4" customWidth="1"/>
+    <col min="2828" max="2831" width="10.25" style="4" customWidth="1"/>
+    <col min="2832" max="2832" width="6.75" style="4" customWidth="1"/>
+    <col min="2833" max="2834" width="10.25" style="4" customWidth="1"/>
+    <col min="2835" max="2835" width="10.375" style="4" customWidth="1"/>
     <col min="2836" max="2839" width="9" style="4" customWidth="1"/>
-    <col min="2840" max="2840" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2841" max="2842" width="8.28515625" style="4" customWidth="1"/>
-    <col min="2843" max="2847" width="6.42578125" style="4" customWidth="1"/>
-    <col min="2848" max="3072" width="6.42578125" style="4"/>
+    <col min="2840" max="2840" width="10.25" style="4" customWidth="1"/>
+    <col min="2841" max="2842" width="8.25" style="4" customWidth="1"/>
+    <col min="2843" max="2847" width="6.375" style="4" customWidth="1"/>
+    <col min="2848" max="3072" width="6.375" style="4"/>
     <col min="3073" max="3073" width="2" style="4" customWidth="1"/>
-    <col min="3074" max="3074" width="7.5703125" style="4" customWidth="1"/>
+    <col min="3074" max="3074" width="7.625" style="4" customWidth="1"/>
     <col min="3075" max="3079" width="9" style="4" customWidth="1"/>
-    <col min="3080" max="3080" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3081" max="3081" width="12.7109375" style="4" customWidth="1"/>
+    <col min="3080" max="3080" width="10.25" style="4" customWidth="1"/>
+    <col min="3081" max="3081" width="12.75" style="4" customWidth="1"/>
     <col min="3082" max="3082" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="3083" max="3083" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="3084" max="3087" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3088" max="3088" width="6.7109375" style="4" customWidth="1"/>
-    <col min="3089" max="3090" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3091" max="3091" width="10.42578125" style="4" customWidth="1"/>
+    <col min="3084" max="3087" width="10.25" style="4" customWidth="1"/>
+    <col min="3088" max="3088" width="6.75" style="4" customWidth="1"/>
+    <col min="3089" max="3090" width="10.25" style="4" customWidth="1"/>
+    <col min="3091" max="3091" width="10.375" style="4" customWidth="1"/>
     <col min="3092" max="3095" width="9" style="4" customWidth="1"/>
-    <col min="3096" max="3096" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3097" max="3098" width="8.28515625" style="4" customWidth="1"/>
-    <col min="3099" max="3103" width="6.42578125" style="4" customWidth="1"/>
-    <col min="3104" max="3328" width="6.42578125" style="4"/>
+    <col min="3096" max="3096" width="10.25" style="4" customWidth="1"/>
+    <col min="3097" max="3098" width="8.25" style="4" customWidth="1"/>
+    <col min="3099" max="3103" width="6.375" style="4" customWidth="1"/>
+    <col min="3104" max="3328" width="6.375" style="4"/>
     <col min="3329" max="3329" width="2" style="4" customWidth="1"/>
-    <col min="3330" max="3330" width="7.5703125" style="4" customWidth="1"/>
+    <col min="3330" max="3330" width="7.625" style="4" customWidth="1"/>
     <col min="3331" max="3335" width="9" style="4" customWidth="1"/>
-    <col min="3336" max="3336" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3337" max="3337" width="12.7109375" style="4" customWidth="1"/>
+    <col min="3336" max="3336" width="10.25" style="4" customWidth="1"/>
+    <col min="3337" max="3337" width="12.75" style="4" customWidth="1"/>
     <col min="3338" max="3338" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="3339" max="3339" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="3340" max="3343" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3344" max="3344" width="6.7109375" style="4" customWidth="1"/>
-    <col min="3345" max="3346" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3347" max="3347" width="10.42578125" style="4" customWidth="1"/>
+    <col min="3340" max="3343" width="10.25" style="4" customWidth="1"/>
+    <col min="3344" max="3344" width="6.75" style="4" customWidth="1"/>
+    <col min="3345" max="3346" width="10.25" style="4" customWidth="1"/>
+    <col min="3347" max="3347" width="10.375" style="4" customWidth="1"/>
     <col min="3348" max="3351" width="9" style="4" customWidth="1"/>
-    <col min="3352" max="3352" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3353" max="3354" width="8.28515625" style="4" customWidth="1"/>
-    <col min="3355" max="3359" width="6.42578125" style="4" customWidth="1"/>
-    <col min="3360" max="3584" width="6.42578125" style="4"/>
+    <col min="3352" max="3352" width="10.25" style="4" customWidth="1"/>
+    <col min="3353" max="3354" width="8.25" style="4" customWidth="1"/>
+    <col min="3355" max="3359" width="6.375" style="4" customWidth="1"/>
+    <col min="3360" max="3584" width="6.375" style="4"/>
     <col min="3585" max="3585" width="2" style="4" customWidth="1"/>
-    <col min="3586" max="3586" width="7.5703125" style="4" customWidth="1"/>
+    <col min="3586" max="3586" width="7.625" style="4" customWidth="1"/>
     <col min="3587" max="3591" width="9" style="4" customWidth="1"/>
-    <col min="3592" max="3592" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3593" max="3593" width="12.7109375" style="4" customWidth="1"/>
+    <col min="3592" max="3592" width="10.25" style="4" customWidth="1"/>
+    <col min="3593" max="3593" width="12.75" style="4" customWidth="1"/>
     <col min="3594" max="3594" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="3595" max="3595" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="3596" max="3599" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3600" max="3600" width="6.7109375" style="4" customWidth="1"/>
-    <col min="3601" max="3602" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3603" max="3603" width="10.42578125" style="4" customWidth="1"/>
+    <col min="3596" max="3599" width="10.25" style="4" customWidth="1"/>
+    <col min="3600" max="3600" width="6.75" style="4" customWidth="1"/>
+    <col min="3601" max="3602" width="10.25" style="4" customWidth="1"/>
+    <col min="3603" max="3603" width="10.375" style="4" customWidth="1"/>
     <col min="3604" max="3607" width="9" style="4" customWidth="1"/>
-    <col min="3608" max="3608" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3609" max="3610" width="8.28515625" style="4" customWidth="1"/>
-    <col min="3611" max="3615" width="6.42578125" style="4" customWidth="1"/>
-    <col min="3616" max="3840" width="6.42578125" style="4"/>
+    <col min="3608" max="3608" width="10.25" style="4" customWidth="1"/>
+    <col min="3609" max="3610" width="8.25" style="4" customWidth="1"/>
+    <col min="3611" max="3615" width="6.375" style="4" customWidth="1"/>
+    <col min="3616" max="3840" width="6.375" style="4"/>
     <col min="3841" max="3841" width="2" style="4" customWidth="1"/>
-    <col min="3842" max="3842" width="7.5703125" style="4" customWidth="1"/>
+    <col min="3842" max="3842" width="7.625" style="4" customWidth="1"/>
     <col min="3843" max="3847" width="9" style="4" customWidth="1"/>
-    <col min="3848" max="3848" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3849" max="3849" width="12.7109375" style="4" customWidth="1"/>
+    <col min="3848" max="3848" width="10.25" style="4" customWidth="1"/>
+    <col min="3849" max="3849" width="12.75" style="4" customWidth="1"/>
     <col min="3850" max="3850" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="3851" max="3851" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="3852" max="3855" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3856" max="3856" width="6.7109375" style="4" customWidth="1"/>
-    <col min="3857" max="3858" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3859" max="3859" width="10.42578125" style="4" customWidth="1"/>
+    <col min="3852" max="3855" width="10.25" style="4" customWidth="1"/>
+    <col min="3856" max="3856" width="6.75" style="4" customWidth="1"/>
+    <col min="3857" max="3858" width="10.25" style="4" customWidth="1"/>
+    <col min="3859" max="3859" width="10.375" style="4" customWidth="1"/>
     <col min="3860" max="3863" width="9" style="4" customWidth="1"/>
-    <col min="3864" max="3864" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3865" max="3866" width="8.28515625" style="4" customWidth="1"/>
-    <col min="3867" max="3871" width="6.42578125" style="4" customWidth="1"/>
-    <col min="3872" max="4096" width="6.42578125" style="4"/>
+    <col min="3864" max="3864" width="10.25" style="4" customWidth="1"/>
+    <col min="3865" max="3866" width="8.25" style="4" customWidth="1"/>
+    <col min="3867" max="3871" width="6.375" style="4" customWidth="1"/>
+    <col min="3872" max="4096" width="6.375" style="4"/>
     <col min="4097" max="4097" width="2" style="4" customWidth="1"/>
-    <col min="4098" max="4098" width="7.5703125" style="4" customWidth="1"/>
+    <col min="4098" max="4098" width="7.625" style="4" customWidth="1"/>
     <col min="4099" max="4103" width="9" style="4" customWidth="1"/>
-    <col min="4104" max="4104" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4105" max="4105" width="12.7109375" style="4" customWidth="1"/>
+    <col min="4104" max="4104" width="10.25" style="4" customWidth="1"/>
+    <col min="4105" max="4105" width="12.75" style="4" customWidth="1"/>
     <col min="4106" max="4106" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="4107" max="4107" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="4108" max="4111" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4112" max="4112" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4113" max="4114" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4115" max="4115" width="10.42578125" style="4" customWidth="1"/>
+    <col min="4108" max="4111" width="10.25" style="4" customWidth="1"/>
+    <col min="4112" max="4112" width="6.75" style="4" customWidth="1"/>
+    <col min="4113" max="4114" width="10.25" style="4" customWidth="1"/>
+    <col min="4115" max="4115" width="10.375" style="4" customWidth="1"/>
     <col min="4116" max="4119" width="9" style="4" customWidth="1"/>
-    <col min="4120" max="4120" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4121" max="4122" width="8.28515625" style="4" customWidth="1"/>
-    <col min="4123" max="4127" width="6.42578125" style="4" customWidth="1"/>
-    <col min="4128" max="4352" width="6.42578125" style="4"/>
+    <col min="4120" max="4120" width="10.25" style="4" customWidth="1"/>
+    <col min="4121" max="4122" width="8.25" style="4" customWidth="1"/>
+    <col min="4123" max="4127" width="6.375" style="4" customWidth="1"/>
+    <col min="4128" max="4352" width="6.375" style="4"/>
     <col min="4353" max="4353" width="2" style="4" customWidth="1"/>
-    <col min="4354" max="4354" width="7.5703125" style="4" customWidth="1"/>
+    <col min="4354" max="4354" width="7.625" style="4" customWidth="1"/>
     <col min="4355" max="4359" width="9" style="4" customWidth="1"/>
-    <col min="4360" max="4360" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4361" max="4361" width="12.7109375" style="4" customWidth="1"/>
+    <col min="4360" max="4360" width="10.25" style="4" customWidth="1"/>
+    <col min="4361" max="4361" width="12.75" style="4" customWidth="1"/>
     <col min="4362" max="4362" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="4363" max="4363" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="4364" max="4367" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4368" max="4368" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4369" max="4370" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4371" max="4371" width="10.42578125" style="4" customWidth="1"/>
+    <col min="4364" max="4367" width="10.25" style="4" customWidth="1"/>
+    <col min="4368" max="4368" width="6.75" style="4" customWidth="1"/>
+    <col min="4369" max="4370" width="10.25" style="4" customWidth="1"/>
+    <col min="4371" max="4371" width="10.375" style="4" customWidth="1"/>
     <col min="4372" max="4375" width="9" style="4" customWidth="1"/>
-    <col min="4376" max="4376" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4377" max="4378" width="8.28515625" style="4" customWidth="1"/>
-    <col min="4379" max="4383" width="6.42578125" style="4" customWidth="1"/>
-    <col min="4384" max="4608" width="6.42578125" style="4"/>
+    <col min="4376" max="4376" width="10.25" style="4" customWidth="1"/>
+    <col min="4377" max="4378" width="8.25" style="4" customWidth="1"/>
+    <col min="4379" max="4383" width="6.375" style="4" customWidth="1"/>
+    <col min="4384" max="4608" width="6.375" style="4"/>
     <col min="4609" max="4609" width="2" style="4" customWidth="1"/>
-    <col min="4610" max="4610" width="7.5703125" style="4" customWidth="1"/>
+    <col min="4610" max="4610" width="7.625" style="4" customWidth="1"/>
     <col min="4611" max="4615" width="9" style="4" customWidth="1"/>
-    <col min="4616" max="4616" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4617" max="4617" width="12.7109375" style="4" customWidth="1"/>
+    <col min="4616" max="4616" width="10.25" style="4" customWidth="1"/>
+    <col min="4617" max="4617" width="12.75" style="4" customWidth="1"/>
     <col min="4618" max="4618" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="4619" max="4619" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="4620" max="4623" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4624" max="4624" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4625" max="4626" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4627" max="4627" width="10.42578125" style="4" customWidth="1"/>
+    <col min="4620" max="4623" width="10.25" style="4" customWidth="1"/>
+    <col min="4624" max="4624" width="6.75" style="4" customWidth="1"/>
+    <col min="4625" max="4626" width="10.25" style="4" customWidth="1"/>
+    <col min="4627" max="4627" width="10.375" style="4" customWidth="1"/>
     <col min="4628" max="4631" width="9" style="4" customWidth="1"/>
-    <col min="4632" max="4632" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4633" max="4634" width="8.28515625" style="4" customWidth="1"/>
-    <col min="4635" max="4639" width="6.42578125" style="4" customWidth="1"/>
-    <col min="4640" max="4864" width="6.42578125" style="4"/>
+    <col min="4632" max="4632" width="10.25" style="4" customWidth="1"/>
+    <col min="4633" max="4634" width="8.25" style="4" customWidth="1"/>
+    <col min="4635" max="4639" width="6.375" style="4" customWidth="1"/>
+    <col min="4640" max="4864" width="6.375" style="4"/>
     <col min="4865" max="4865" width="2" style="4" customWidth="1"/>
-    <col min="4866" max="4866" width="7.5703125" style="4" customWidth="1"/>
+    <col min="4866" max="4866" width="7.625" style="4" customWidth="1"/>
     <col min="4867" max="4871" width="9" style="4" customWidth="1"/>
-    <col min="4872" max="4872" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4873" max="4873" width="12.7109375" style="4" customWidth="1"/>
+    <col min="4872" max="4872" width="10.25" style="4" customWidth="1"/>
+    <col min="4873" max="4873" width="12.75" style="4" customWidth="1"/>
     <col min="4874" max="4874" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="4875" max="4875" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="4876" max="4879" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4880" max="4880" width="6.7109375" style="4" customWidth="1"/>
-    <col min="4881" max="4882" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4883" max="4883" width="10.42578125" style="4" customWidth="1"/>
+    <col min="4876" max="4879" width="10.25" style="4" customWidth="1"/>
+    <col min="4880" max="4880" width="6.75" style="4" customWidth="1"/>
+    <col min="4881" max="4882" width="10.25" style="4" customWidth="1"/>
+    <col min="4883" max="4883" width="10.375" style="4" customWidth="1"/>
     <col min="4884" max="4887" width="9" style="4" customWidth="1"/>
-    <col min="4888" max="4888" width="10.28515625" style="4" customWidth="1"/>
-    <col min="4889" max="4890" width="8.28515625" style="4" customWidth="1"/>
-    <col min="4891" max="4895" width="6.42578125" style="4" customWidth="1"/>
-    <col min="4896" max="5120" width="6.42578125" style="4"/>
+    <col min="4888" max="4888" width="10.25" style="4" customWidth="1"/>
+    <col min="4889" max="4890" width="8.25" style="4" customWidth="1"/>
+    <col min="4891" max="4895" width="6.375" style="4" customWidth="1"/>
+    <col min="4896" max="5120" width="6.375" style="4"/>
     <col min="5121" max="5121" width="2" style="4" customWidth="1"/>
-    <col min="5122" max="5122" width="7.5703125" style="4" customWidth="1"/>
+    <col min="5122" max="5122" width="7.625" style="4" customWidth="1"/>
     <col min="5123" max="5127" width="9" style="4" customWidth="1"/>
-    <col min="5128" max="5128" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5129" max="5129" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5128" max="5128" width="10.25" style="4" customWidth="1"/>
+    <col min="5129" max="5129" width="12.75" style="4" customWidth="1"/>
     <col min="5130" max="5130" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="5131" max="5131" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="5132" max="5135" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5136" max="5136" width="6.7109375" style="4" customWidth="1"/>
-    <col min="5137" max="5138" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5139" max="5139" width="10.42578125" style="4" customWidth="1"/>
+    <col min="5132" max="5135" width="10.25" style="4" customWidth="1"/>
+    <col min="5136" max="5136" width="6.75" style="4" customWidth="1"/>
+    <col min="5137" max="5138" width="10.25" style="4" customWidth="1"/>
+    <col min="5139" max="5139" width="10.375" style="4" customWidth="1"/>
     <col min="5140" max="5143" width="9" style="4" customWidth="1"/>
-    <col min="5144" max="5144" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5145" max="5146" width="8.28515625" style="4" customWidth="1"/>
-    <col min="5147" max="5151" width="6.42578125" style="4" customWidth="1"/>
-    <col min="5152" max="5376" width="6.42578125" style="4"/>
+    <col min="5144" max="5144" width="10.25" style="4" customWidth="1"/>
+    <col min="5145" max="5146" width="8.25" style="4" customWidth="1"/>
+    <col min="5147" max="5151" width="6.375" style="4" customWidth="1"/>
+    <col min="5152" max="5376" width="6.375" style="4"/>
     <col min="5377" max="5377" width="2" style="4" customWidth="1"/>
-    <col min="5378" max="5378" width="7.5703125" style="4" customWidth="1"/>
+    <col min="5378" max="5378" width="7.625" style="4" customWidth="1"/>
     <col min="5379" max="5383" width="9" style="4" customWidth="1"/>
-    <col min="5384" max="5384" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5385" max="5385" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5384" max="5384" width="10.25" style="4" customWidth="1"/>
+    <col min="5385" max="5385" width="12.75" style="4" customWidth="1"/>
     <col min="5386" max="5386" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="5387" max="5387" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="5388" max="5391" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5392" max="5392" width="6.7109375" style="4" customWidth="1"/>
-    <col min="5393" max="5394" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5395" max="5395" width="10.42578125" style="4" customWidth="1"/>
+    <col min="5388" max="5391" width="10.25" style="4" customWidth="1"/>
+    <col min="5392" max="5392" width="6.75" style="4" customWidth="1"/>
+    <col min="5393" max="5394" width="10.25" style="4" customWidth="1"/>
+    <col min="5395" max="5395" width="10.375" style="4" customWidth="1"/>
     <col min="5396" max="5399" width="9" style="4" customWidth="1"/>
-    <col min="5400" max="5400" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5401" max="5402" width="8.28515625" style="4" customWidth="1"/>
-    <col min="5403" max="5407" width="6.42578125" style="4" customWidth="1"/>
-    <col min="5408" max="5632" width="6.42578125" style="4"/>
+    <col min="5400" max="5400" width="10.25" style="4" customWidth="1"/>
+    <col min="5401" max="5402" width="8.25" style="4" customWidth="1"/>
+    <col min="5403" max="5407" width="6.375" style="4" customWidth="1"/>
+    <col min="5408" max="5632" width="6.375" style="4"/>
     <col min="5633" max="5633" width="2" style="4" customWidth="1"/>
-    <col min="5634" max="5634" width="7.5703125" style="4" customWidth="1"/>
+    <col min="5634" max="5634" width="7.625" style="4" customWidth="1"/>
     <col min="5635" max="5639" width="9" style="4" customWidth="1"/>
-    <col min="5640" max="5640" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5641" max="5641" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5640" max="5640" width="10.25" style="4" customWidth="1"/>
+    <col min="5641" max="5641" width="12.75" style="4" customWidth="1"/>
     <col min="5642" max="5642" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="5643" max="5643" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="5644" max="5647" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5648" max="5648" width="6.7109375" style="4" customWidth="1"/>
-    <col min="5649" max="5650" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5651" max="5651" width="10.42578125" style="4" customWidth="1"/>
+    <col min="5644" max="5647" width="10.25" style="4" customWidth="1"/>
+    <col min="5648" max="5648" width="6.75" style="4" customWidth="1"/>
+    <col min="5649" max="5650" width="10.25" style="4" customWidth="1"/>
+    <col min="5651" max="5651" width="10.375" style="4" customWidth="1"/>
     <col min="5652" max="5655" width="9" style="4" customWidth="1"/>
-    <col min="5656" max="5656" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5657" max="5658" width="8.28515625" style="4" customWidth="1"/>
-    <col min="5659" max="5663" width="6.42578125" style="4" customWidth="1"/>
-    <col min="5664" max="5888" width="6.42578125" style="4"/>
+    <col min="5656" max="5656" width="10.25" style="4" customWidth="1"/>
+    <col min="5657" max="5658" width="8.25" style="4" customWidth="1"/>
+    <col min="5659" max="5663" width="6.375" style="4" customWidth="1"/>
+    <col min="5664" max="5888" width="6.375" style="4"/>
     <col min="5889" max="5889" width="2" style="4" customWidth="1"/>
-    <col min="5890" max="5890" width="7.5703125" style="4" customWidth="1"/>
+    <col min="5890" max="5890" width="7.625" style="4" customWidth="1"/>
     <col min="5891" max="5895" width="9" style="4" customWidth="1"/>
-    <col min="5896" max="5896" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5897" max="5897" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5896" max="5896" width="10.25" style="4" customWidth="1"/>
+    <col min="5897" max="5897" width="12.75" style="4" customWidth="1"/>
     <col min="5898" max="5898" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="5899" max="5899" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="5900" max="5903" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5904" max="5904" width="6.7109375" style="4" customWidth="1"/>
-    <col min="5905" max="5906" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5907" max="5907" width="10.42578125" style="4" customWidth="1"/>
+    <col min="5900" max="5903" width="10.25" style="4" customWidth="1"/>
+    <col min="5904" max="5904" width="6.75" style="4" customWidth="1"/>
+    <col min="5905" max="5906" width="10.25" style="4" customWidth="1"/>
+    <col min="5907" max="5907" width="10.375" style="4" customWidth="1"/>
     <col min="5908" max="5911" width="9" style="4" customWidth="1"/>
-    <col min="5912" max="5912" width="10.28515625" style="4" customWidth="1"/>
-    <col min="5913" max="5914" width="8.28515625" style="4" customWidth="1"/>
-    <col min="5915" max="5919" width="6.42578125" style="4" customWidth="1"/>
-    <col min="5920" max="6144" width="6.42578125" style="4"/>
+    <col min="5912" max="5912" width="10.25" style="4" customWidth="1"/>
+    <col min="5913" max="5914" width="8.25" style="4" customWidth="1"/>
+    <col min="5915" max="5919" width="6.375" style="4" customWidth="1"/>
+    <col min="5920" max="6144" width="6.375" style="4"/>
     <col min="6145" max="6145" width="2" style="4" customWidth="1"/>
-    <col min="6146" max="6146" width="7.5703125" style="4" customWidth="1"/>
+    <col min="6146" max="6146" width="7.625" style="4" customWidth="1"/>
     <col min="6147" max="6151" width="9" style="4" customWidth="1"/>
-    <col min="6152" max="6152" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6153" max="6153" width="12.7109375" style="4" customWidth="1"/>
+    <col min="6152" max="6152" width="10.25" style="4" customWidth="1"/>
+    <col min="6153" max="6153" width="12.75" style="4" customWidth="1"/>
     <col min="6154" max="6154" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="6155" max="6155" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="6156" max="6159" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6160" max="6160" width="6.7109375" style="4" customWidth="1"/>
-    <col min="6161" max="6162" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6163" max="6163" width="10.42578125" style="4" customWidth="1"/>
+    <col min="6156" max="6159" width="10.25" style="4" customWidth="1"/>
+    <col min="6160" max="6160" width="6.75" style="4" customWidth="1"/>
+    <col min="6161" max="6162" width="10.25" style="4" customWidth="1"/>
+    <col min="6163" max="6163" width="10.375" style="4" customWidth="1"/>
     <col min="6164" max="6167" width="9" style="4" customWidth="1"/>
-    <col min="6168" max="6168" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6169" max="6170" width="8.28515625" style="4" customWidth="1"/>
-    <col min="6171" max="6175" width="6.42578125" style="4" customWidth="1"/>
-    <col min="6176" max="6400" width="6.42578125" style="4"/>
+    <col min="6168" max="6168" width="10.25" style="4" customWidth="1"/>
+    <col min="6169" max="6170" width="8.25" style="4" customWidth="1"/>
+    <col min="6171" max="6175" width="6.375" style="4" customWidth="1"/>
+    <col min="6176" max="6400" width="6.375" style="4"/>
     <col min="6401" max="6401" width="2" style="4" customWidth="1"/>
-    <col min="6402" max="6402" width="7.5703125" style="4" customWidth="1"/>
+    <col min="6402" max="6402" width="7.625" style="4" customWidth="1"/>
     <col min="6403" max="6407" width="9" style="4" customWidth="1"/>
-    <col min="6408" max="6408" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6409" max="6409" width="12.7109375" style="4" customWidth="1"/>
+    <col min="6408" max="6408" width="10.25" style="4" customWidth="1"/>
+    <col min="6409" max="6409" width="12.75" style="4" customWidth="1"/>
     <col min="6410" max="6410" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="6411" max="6411" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="6412" max="6415" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6416" max="6416" width="6.7109375" style="4" customWidth="1"/>
-    <col min="6417" max="6418" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6419" max="6419" width="10.42578125" style="4" customWidth="1"/>
+    <col min="6412" max="6415" width="10.25" style="4" customWidth="1"/>
+    <col min="6416" max="6416" width="6.75" style="4" customWidth="1"/>
+    <col min="6417" max="6418" width="10.25" style="4" customWidth="1"/>
+    <col min="6419" max="6419" width="10.375" style="4" customWidth="1"/>
     <col min="6420" max="6423" width="9" style="4" customWidth="1"/>
-    <col min="6424" max="6424" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6425" max="6426" width="8.28515625" style="4" customWidth="1"/>
-    <col min="6427" max="6431" width="6.42578125" style="4" customWidth="1"/>
-    <col min="6432" max="6656" width="6.42578125" style="4"/>
+    <col min="6424" max="6424" width="10.25" style="4" customWidth="1"/>
+    <col min="6425" max="6426" width="8.25" style="4" customWidth="1"/>
+    <col min="6427" max="6431" width="6.375" style="4" customWidth="1"/>
+    <col min="6432" max="6656" width="6.375" style="4"/>
     <col min="6657" max="6657" width="2" style="4" customWidth="1"/>
-    <col min="6658" max="6658" width="7.5703125" style="4" customWidth="1"/>
+    <col min="6658" max="6658" width="7.625" style="4" customWidth="1"/>
     <col min="6659" max="6663" width="9" style="4" customWidth="1"/>
-    <col min="6664" max="6664" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6665" max="6665" width="12.7109375" style="4" customWidth="1"/>
+    <col min="6664" max="6664" width="10.25" style="4" customWidth="1"/>
+    <col min="6665" max="6665" width="12.75" style="4" customWidth="1"/>
     <col min="6666" max="6666" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="6667" max="6667" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="6668" max="6671" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6672" max="6672" width="6.7109375" style="4" customWidth="1"/>
-    <col min="6673" max="6674" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6675" max="6675" width="10.42578125" style="4" customWidth="1"/>
+    <col min="6668" max="6671" width="10.25" style="4" customWidth="1"/>
+    <col min="6672" max="6672" width="6.75" style="4" customWidth="1"/>
+    <col min="6673" max="6674" width="10.25" style="4" customWidth="1"/>
+    <col min="6675" max="6675" width="10.375" style="4" customWidth="1"/>
     <col min="6676" max="6679" width="9" style="4" customWidth="1"/>
-    <col min="6680" max="6680" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6681" max="6682" width="8.28515625" style="4" customWidth="1"/>
-    <col min="6683" max="6687" width="6.42578125" style="4" customWidth="1"/>
-    <col min="6688" max="6912" width="6.42578125" style="4"/>
+    <col min="6680" max="6680" width="10.25" style="4" customWidth="1"/>
+    <col min="6681" max="6682" width="8.25" style="4" customWidth="1"/>
+    <col min="6683" max="6687" width="6.375" style="4" customWidth="1"/>
+    <col min="6688" max="6912" width="6.375" style="4"/>
     <col min="6913" max="6913" width="2" style="4" customWidth="1"/>
-    <col min="6914" max="6914" width="7.5703125" style="4" customWidth="1"/>
+    <col min="6914" max="6914" width="7.625" style="4" customWidth="1"/>
     <col min="6915" max="6919" width="9" style="4" customWidth="1"/>
-    <col min="6920" max="6920" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6921" max="6921" width="12.7109375" style="4" customWidth="1"/>
+    <col min="6920" max="6920" width="10.25" style="4" customWidth="1"/>
+    <col min="6921" max="6921" width="12.75" style="4" customWidth="1"/>
     <col min="6922" max="6922" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="6923" max="6923" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="6924" max="6927" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6928" max="6928" width="6.7109375" style="4" customWidth="1"/>
-    <col min="6929" max="6930" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6931" max="6931" width="10.42578125" style="4" customWidth="1"/>
+    <col min="6924" max="6927" width="10.25" style="4" customWidth="1"/>
+    <col min="6928" max="6928" width="6.75" style="4" customWidth="1"/>
+    <col min="6929" max="6930" width="10.25" style="4" customWidth="1"/>
+    <col min="6931" max="6931" width="10.375" style="4" customWidth="1"/>
     <col min="6932" max="6935" width="9" style="4" customWidth="1"/>
-    <col min="6936" max="6936" width="10.28515625" style="4" customWidth="1"/>
-    <col min="6937" max="6938" width="8.28515625" style="4" customWidth="1"/>
-    <col min="6939" max="6943" width="6.42578125" style="4" customWidth="1"/>
-    <col min="6944" max="7168" width="6.42578125" style="4"/>
+    <col min="6936" max="6936" width="10.25" style="4" customWidth="1"/>
+    <col min="6937" max="6938" width="8.25" style="4" customWidth="1"/>
+    <col min="6939" max="6943" width="6.375" style="4" customWidth="1"/>
+    <col min="6944" max="7168" width="6.375" style="4"/>
     <col min="7169" max="7169" width="2" style="4" customWidth="1"/>
-    <col min="7170" max="7170" width="7.5703125" style="4" customWidth="1"/>
+    <col min="7170" max="7170" width="7.625" style="4" customWidth="1"/>
     <col min="7171" max="7175" width="9" style="4" customWidth="1"/>
-    <col min="7176" max="7176" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7177" max="7177" width="12.7109375" style="4" customWidth="1"/>
+    <col min="7176" max="7176" width="10.25" style="4" customWidth="1"/>
+    <col min="7177" max="7177" width="12.75" style="4" customWidth="1"/>
     <col min="7178" max="7178" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="7179" max="7179" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="7180" max="7183" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7184" max="7184" width="6.7109375" style="4" customWidth="1"/>
-    <col min="7185" max="7186" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7187" max="7187" width="10.42578125" style="4" customWidth="1"/>
+    <col min="7180" max="7183" width="10.25" style="4" customWidth="1"/>
+    <col min="7184" max="7184" width="6.75" style="4" customWidth="1"/>
+    <col min="7185" max="7186" width="10.25" style="4" customWidth="1"/>
+    <col min="7187" max="7187" width="10.375" style="4" customWidth="1"/>
     <col min="7188" max="7191" width="9" style="4" customWidth="1"/>
-    <col min="7192" max="7192" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7193" max="7194" width="8.28515625" style="4" customWidth="1"/>
-    <col min="7195" max="7199" width="6.42578125" style="4" customWidth="1"/>
-    <col min="7200" max="7424" width="6.42578125" style="4"/>
+    <col min="7192" max="7192" width="10.25" style="4" customWidth="1"/>
+    <col min="7193" max="7194" width="8.25" style="4" customWidth="1"/>
+    <col min="7195" max="7199" width="6.375" style="4" customWidth="1"/>
+    <col min="7200" max="7424" width="6.375" style="4"/>
     <col min="7425" max="7425" width="2" style="4" customWidth="1"/>
-    <col min="7426" max="7426" width="7.5703125" style="4" customWidth="1"/>
+    <col min="7426" max="7426" width="7.625" style="4" customWidth="1"/>
     <col min="7427" max="7431" width="9" style="4" customWidth="1"/>
-    <col min="7432" max="7432" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7433" max="7433" width="12.7109375" style="4" customWidth="1"/>
+    <col min="7432" max="7432" width="10.25" style="4" customWidth="1"/>
+    <col min="7433" max="7433" width="12.75" style="4" customWidth="1"/>
     <col min="7434" max="7434" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="7435" max="7435" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="7436" max="7439" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7440" max="7440" width="6.7109375" style="4" customWidth="1"/>
-    <col min="7441" max="7442" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7443" max="7443" width="10.42578125" style="4" customWidth="1"/>
+    <col min="7436" max="7439" width="10.25" style="4" customWidth="1"/>
+    <col min="7440" max="7440" width="6.75" style="4" customWidth="1"/>
+    <col min="7441" max="7442" width="10.25" style="4" customWidth="1"/>
+    <col min="7443" max="7443" width="10.375" style="4" customWidth="1"/>
     <col min="7444" max="7447" width="9" style="4" customWidth="1"/>
-    <col min="7448" max="7448" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7449" max="7450" width="8.28515625" style="4" customWidth="1"/>
-    <col min="7451" max="7455" width="6.42578125" style="4" customWidth="1"/>
-    <col min="7456" max="7680" width="6.42578125" style="4"/>
+    <col min="7448" max="7448" width="10.25" style="4" customWidth="1"/>
+    <col min="7449" max="7450" width="8.25" style="4" customWidth="1"/>
+    <col min="7451" max="7455" width="6.375" style="4" customWidth="1"/>
+    <col min="7456" max="7680" width="6.375" style="4"/>
     <col min="7681" max="7681" width="2" style="4" customWidth="1"/>
-    <col min="7682" max="7682" width="7.5703125" style="4" customWidth="1"/>
+    <col min="7682" max="7682" width="7.625" style="4" customWidth="1"/>
     <col min="7683" max="7687" width="9" style="4" customWidth="1"/>
-    <col min="7688" max="7688" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7689" max="7689" width="12.7109375" style="4" customWidth="1"/>
+    <col min="7688" max="7688" width="10.25" style="4" customWidth="1"/>
+    <col min="7689" max="7689" width="12.75" style="4" customWidth="1"/>
     <col min="7690" max="7690" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="7691" max="7691" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="7692" max="7695" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7696" max="7696" width="6.7109375" style="4" customWidth="1"/>
-    <col min="7697" max="7698" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7699" max="7699" width="10.42578125" style="4" customWidth="1"/>
+    <col min="7692" max="7695" width="10.25" style="4" customWidth="1"/>
+    <col min="7696" max="7696" width="6.75" style="4" customWidth="1"/>
+    <col min="7697" max="7698" width="10.25" style="4" customWidth="1"/>
+    <col min="7699" max="7699" width="10.375" style="4" customWidth="1"/>
     <col min="7700" max="7703" width="9" style="4" customWidth="1"/>
-    <col min="7704" max="7704" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7705" max="7706" width="8.28515625" style="4" customWidth="1"/>
-    <col min="7707" max="7711" width="6.42578125" style="4" customWidth="1"/>
-    <col min="7712" max="7936" width="6.42578125" style="4"/>
+    <col min="7704" max="7704" width="10.25" style="4" customWidth="1"/>
+    <col min="7705" max="7706" width="8.25" style="4" customWidth="1"/>
+    <col min="7707" max="7711" width="6.375" style="4" customWidth="1"/>
+    <col min="7712" max="7936" width="6.375" style="4"/>
     <col min="7937" max="7937" width="2" style="4" customWidth="1"/>
-    <col min="7938" max="7938" width="7.5703125" style="4" customWidth="1"/>
+    <col min="7938" max="7938" width="7.625" style="4" customWidth="1"/>
     <col min="7939" max="7943" width="9" style="4" customWidth="1"/>
-    <col min="7944" max="7944" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7945" max="7945" width="12.7109375" style="4" customWidth="1"/>
+    <col min="7944" max="7944" width="10.25" style="4" customWidth="1"/>
+    <col min="7945" max="7945" width="12.75" style="4" customWidth="1"/>
     <col min="7946" max="7946" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="7947" max="7947" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="7948" max="7951" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7952" max="7952" width="6.7109375" style="4" customWidth="1"/>
-    <col min="7953" max="7954" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7955" max="7955" width="10.42578125" style="4" customWidth="1"/>
+    <col min="7948" max="7951" width="10.25" style="4" customWidth="1"/>
+    <col min="7952" max="7952" width="6.75" style="4" customWidth="1"/>
+    <col min="7953" max="7954" width="10.25" style="4" customWidth="1"/>
+    <col min="7955" max="7955" width="10.375" style="4" customWidth="1"/>
     <col min="7956" max="7959" width="9" style="4" customWidth="1"/>
-    <col min="7960" max="7960" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7961" max="7962" width="8.28515625" style="4" customWidth="1"/>
-    <col min="7963" max="7967" width="6.42578125" style="4" customWidth="1"/>
-    <col min="7968" max="8192" width="6.42578125" style="4"/>
+    <col min="7960" max="7960" width="10.25" style="4" customWidth="1"/>
+    <col min="7961" max="7962" width="8.25" style="4" customWidth="1"/>
+    <col min="7963" max="7967" width="6.375" style="4" customWidth="1"/>
+    <col min="7968" max="8192" width="6.375" style="4"/>
     <col min="8193" max="8193" width="2" style="4" customWidth="1"/>
-    <col min="8194" max="8194" width="7.5703125" style="4" customWidth="1"/>
+    <col min="8194" max="8194" width="7.625" style="4" customWidth="1"/>
     <col min="8195" max="8199" width="9" style="4" customWidth="1"/>
-    <col min="8200" max="8200" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8201" max="8201" width="12.7109375" style="4" customWidth="1"/>
+    <col min="8200" max="8200" width="10.25" style="4" customWidth="1"/>
+    <col min="8201" max="8201" width="12.75" style="4" customWidth="1"/>
     <col min="8202" max="8202" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="8203" max="8203" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="8204" max="8207" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8208" max="8208" width="6.7109375" style="4" customWidth="1"/>
-    <col min="8209" max="8210" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8211" max="8211" width="10.42578125" style="4" customWidth="1"/>
+    <col min="8204" max="8207" width="10.25" style="4" customWidth="1"/>
+    <col min="8208" max="8208" width="6.75" style="4" customWidth="1"/>
+    <col min="8209" max="8210" width="10.25" style="4" customWidth="1"/>
+    <col min="8211" max="8211" width="10.375" style="4" customWidth="1"/>
     <col min="8212" max="8215" width="9" style="4" customWidth="1"/>
-    <col min="8216" max="8216" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8217" max="8218" width="8.28515625" style="4" customWidth="1"/>
-    <col min="8219" max="8223" width="6.42578125" style="4" customWidth="1"/>
-    <col min="8224" max="8448" width="6.42578125" style="4"/>
+    <col min="8216" max="8216" width="10.25" style="4" customWidth="1"/>
+    <col min="8217" max="8218" width="8.25" style="4" customWidth="1"/>
+    <col min="8219" max="8223" width="6.375" style="4" customWidth="1"/>
+    <col min="8224" max="8448" width="6.375" style="4"/>
     <col min="8449" max="8449" width="2" style="4" customWidth="1"/>
-    <col min="8450" max="8450" width="7.5703125" style="4" customWidth="1"/>
+    <col min="8450" max="8450" width="7.625" style="4" customWidth="1"/>
     <col min="8451" max="8455" width="9" style="4" customWidth="1"/>
-    <col min="8456" max="8456" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8457" max="8457" width="12.7109375" style="4" customWidth="1"/>
+    <col min="8456" max="8456" width="10.25" style="4" customWidth="1"/>
+    <col min="8457" max="8457" width="12.75" style="4" customWidth="1"/>
     <col min="8458" max="8458" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="8459" max="8459" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="8460" max="8463" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8464" max="8464" width="6.7109375" style="4" customWidth="1"/>
-    <col min="8465" max="8466" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8467" max="8467" width="10.42578125" style="4" customWidth="1"/>
+    <col min="8460" max="8463" width="10.25" style="4" customWidth="1"/>
+    <col min="8464" max="8464" width="6.75" style="4" customWidth="1"/>
+    <col min="8465" max="8466" width="10.25" style="4" customWidth="1"/>
+    <col min="8467" max="8467" width="10.375" style="4" customWidth="1"/>
     <col min="8468" max="8471" width="9" style="4" customWidth="1"/>
-    <col min="8472" max="8472" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8473" max="8474" width="8.28515625" style="4" customWidth="1"/>
-    <col min="8475" max="8479" width="6.42578125" style="4" customWidth="1"/>
-    <col min="8480" max="8704" width="6.42578125" style="4"/>
+    <col min="8472" max="8472" width="10.25" style="4" customWidth="1"/>
+    <col min="8473" max="8474" width="8.25" style="4" customWidth="1"/>
+    <col min="8475" max="8479" width="6.375" style="4" customWidth="1"/>
+    <col min="8480" max="8704" width="6.375" style="4"/>
     <col min="8705" max="8705" width="2" style="4" customWidth="1"/>
-    <col min="8706" max="8706" width="7.5703125" style="4" customWidth="1"/>
+    <col min="8706" max="8706" width="7.625" style="4" customWidth="1"/>
     <col min="8707" max="8711" width="9" style="4" customWidth="1"/>
-    <col min="8712" max="8712" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8713" max="8713" width="12.7109375" style="4" customWidth="1"/>
+    <col min="8712" max="8712" width="10.25" style="4" customWidth="1"/>
+    <col min="8713" max="8713" width="12.75" style="4" customWidth="1"/>
     <col min="8714" max="8714" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="8715" max="8715" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="8716" max="8719" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8720" max="8720" width="6.7109375" style="4" customWidth="1"/>
-    <col min="8721" max="8722" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8723" max="8723" width="10.42578125" style="4" customWidth="1"/>
+    <col min="8716" max="8719" width="10.25" style="4" customWidth="1"/>
+    <col min="8720" max="8720" width="6.75" style="4" customWidth="1"/>
+    <col min="8721" max="8722" width="10.25" style="4" customWidth="1"/>
+    <col min="8723" max="8723" width="10.375" style="4" customWidth="1"/>
     <col min="8724" max="8727" width="9" style="4" customWidth="1"/>
-    <col min="8728" max="8728" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8729" max="8730" width="8.28515625" style="4" customWidth="1"/>
-    <col min="8731" max="8735" width="6.42578125" style="4" customWidth="1"/>
-    <col min="8736" max="8960" width="6.42578125" style="4"/>
+    <col min="8728" max="8728" width="10.25" style="4" customWidth="1"/>
+    <col min="8729" max="8730" width="8.25" style="4" customWidth="1"/>
+    <col min="8731" max="8735" width="6.375" style="4" customWidth="1"/>
+    <col min="8736" max="8960" width="6.375" style="4"/>
     <col min="8961" max="8961" width="2" style="4" customWidth="1"/>
-    <col min="8962" max="8962" width="7.5703125" style="4" customWidth="1"/>
+    <col min="8962" max="8962" width="7.625" style="4" customWidth="1"/>
     <col min="8963" max="8967" width="9" style="4" customWidth="1"/>
-    <col min="8968" max="8968" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8969" max="8969" width="12.7109375" style="4" customWidth="1"/>
+    <col min="8968" max="8968" width="10.25" style="4" customWidth="1"/>
+    <col min="8969" max="8969" width="12.75" style="4" customWidth="1"/>
     <col min="8970" max="8970" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="8971" max="8971" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="8972" max="8975" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8976" max="8976" width="6.7109375" style="4" customWidth="1"/>
-    <col min="8977" max="8978" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8979" max="8979" width="10.42578125" style="4" customWidth="1"/>
+    <col min="8972" max="8975" width="10.25" style="4" customWidth="1"/>
+    <col min="8976" max="8976" width="6.75" style="4" customWidth="1"/>
+    <col min="8977" max="8978" width="10.25" style="4" customWidth="1"/>
+    <col min="8979" max="8979" width="10.375" style="4" customWidth="1"/>
     <col min="8980" max="8983" width="9" style="4" customWidth="1"/>
-    <col min="8984" max="8984" width="10.28515625" style="4" customWidth="1"/>
-    <col min="8985" max="8986" width="8.28515625" style="4" customWidth="1"/>
-    <col min="8987" max="8991" width="6.42578125" style="4" customWidth="1"/>
-    <col min="8992" max="9216" width="6.42578125" style="4"/>
+    <col min="8984" max="8984" width="10.25" style="4" customWidth="1"/>
+    <col min="8985" max="8986" width="8.25" style="4" customWidth="1"/>
+    <col min="8987" max="8991" width="6.375" style="4" customWidth="1"/>
+    <col min="8992" max="9216" width="6.375" style="4"/>
     <col min="9217" max="9217" width="2" style="4" customWidth="1"/>
-    <col min="9218" max="9218" width="7.5703125" style="4" customWidth="1"/>
+    <col min="9218" max="9218" width="7.625" style="4" customWidth="1"/>
     <col min="9219" max="9223" width="9" style="4" customWidth="1"/>
-    <col min="9224" max="9224" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9225" max="9225" width="12.7109375" style="4" customWidth="1"/>
+    <col min="9224" max="9224" width="10.25" style="4" customWidth="1"/>
+    <col min="9225" max="9225" width="12.75" style="4" customWidth="1"/>
     <col min="9226" max="9226" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="9227" max="9227" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="9228" max="9231" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9232" max="9232" width="6.7109375" style="4" customWidth="1"/>
-    <col min="9233" max="9234" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9235" max="9235" width="10.42578125" style="4" customWidth="1"/>
+    <col min="9228" max="9231" width="10.25" style="4" customWidth="1"/>
+    <col min="9232" max="9232" width="6.75" style="4" customWidth="1"/>
+    <col min="9233" max="9234" width="10.25" style="4" customWidth="1"/>
+    <col min="9235" max="9235" width="10.375" style="4" customWidth="1"/>
     <col min="9236" max="9239" width="9" style="4" customWidth="1"/>
-    <col min="9240" max="9240" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9241" max="9242" width="8.28515625" style="4" customWidth="1"/>
-    <col min="9243" max="9247" width="6.42578125" style="4" customWidth="1"/>
-    <col min="9248" max="9472" width="6.42578125" style="4"/>
+    <col min="9240" max="9240" width="10.25" style="4" customWidth="1"/>
+    <col min="9241" max="9242" width="8.25" style="4" customWidth="1"/>
+    <col min="9243" max="9247" width="6.375" style="4" customWidth="1"/>
+    <col min="9248" max="9472" width="6.375" style="4"/>
     <col min="9473" max="9473" width="2" style="4" customWidth="1"/>
-    <col min="9474" max="9474" width="7.5703125" style="4" customWidth="1"/>
+    <col min="9474" max="9474" width="7.625" style="4" customWidth="1"/>
     <col min="9475" max="9479" width="9" style="4" customWidth="1"/>
-    <col min="9480" max="9480" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9481" max="9481" width="12.7109375" style="4" customWidth="1"/>
+    <col min="9480" max="9480" width="10.25" style="4" customWidth="1"/>
+    <col min="9481" max="9481" width="12.75" style="4" customWidth="1"/>
     <col min="9482" max="9482" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="9483" max="9483" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="9484" max="9487" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9488" max="9488" width="6.7109375" style="4" customWidth="1"/>
-    <col min="9489" max="9490" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9491" max="9491" width="10.42578125" style="4" customWidth="1"/>
+    <col min="9484" max="9487" width="10.25" style="4" customWidth="1"/>
+    <col min="9488" max="9488" width="6.75" style="4" customWidth="1"/>
+    <col min="9489" max="9490" width="10.25" style="4" customWidth="1"/>
+    <col min="9491" max="9491" width="10.375" style="4" customWidth="1"/>
     <col min="9492" max="9495" width="9" style="4" customWidth="1"/>
-    <col min="9496" max="9496" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9497" max="9498" width="8.28515625" style="4" customWidth="1"/>
-    <col min="9499" max="9503" width="6.42578125" style="4" customWidth="1"/>
-    <col min="9504" max="9728" width="6.42578125" style="4"/>
+    <col min="9496" max="9496" width="10.25" style="4" customWidth="1"/>
+    <col min="9497" max="9498" width="8.25" style="4" customWidth="1"/>
+    <col min="9499" max="9503" width="6.375" style="4" customWidth="1"/>
+    <col min="9504" max="9728" width="6.375" style="4"/>
     <col min="9729" max="9729" width="2" style="4" customWidth="1"/>
-    <col min="9730" max="9730" width="7.5703125" style="4" customWidth="1"/>
+    <col min="9730" max="9730" width="7.625" style="4" customWidth="1"/>
     <col min="9731" max="9735" width="9" style="4" customWidth="1"/>
-    <col min="9736" max="9736" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9737" max="9737" width="12.7109375" style="4" customWidth="1"/>
+    <col min="9736" max="9736" width="10.25" style="4" customWidth="1"/>
+    <col min="9737" max="9737" width="12.75" style="4" customWidth="1"/>
     <col min="9738" max="9738" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="9739" max="9739" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="9740" max="9743" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9744" max="9744" width="6.7109375" style="4" customWidth="1"/>
-    <col min="9745" max="9746" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9747" max="9747" width="10.42578125" style="4" customWidth="1"/>
+    <col min="9740" max="9743" width="10.25" style="4" customWidth="1"/>
+    <col min="9744" max="9744" width="6.75" style="4" customWidth="1"/>
+    <col min="9745" max="9746" width="10.25" style="4" customWidth="1"/>
+    <col min="9747" max="9747" width="10.375" style="4" customWidth="1"/>
     <col min="9748" max="9751" width="9" style="4" customWidth="1"/>
-    <col min="9752" max="9752" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9753" max="9754" width="8.28515625" style="4" customWidth="1"/>
-    <col min="9755" max="9759" width="6.42578125" style="4" customWidth="1"/>
-    <col min="9760" max="9984" width="6.42578125" style="4"/>
+    <col min="9752" max="9752" width="10.25" style="4" customWidth="1"/>
+    <col min="9753" max="9754" width="8.25" style="4" customWidth="1"/>
+    <col min="9755" max="9759" width="6.375" style="4" customWidth="1"/>
+    <col min="9760" max="9984" width="6.375" style="4"/>
     <col min="9985" max="9985" width="2" style="4" customWidth="1"/>
-    <col min="9986" max="9986" width="7.5703125" style="4" customWidth="1"/>
+    <col min="9986" max="9986" width="7.625" style="4" customWidth="1"/>
     <col min="9987" max="9991" width="9" style="4" customWidth="1"/>
-    <col min="9992" max="9992" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9993" max="9993" width="12.7109375" style="4" customWidth="1"/>
+    <col min="9992" max="9992" width="10.25" style="4" customWidth="1"/>
+    <col min="9993" max="9993" width="12.75" style="4" customWidth="1"/>
     <col min="9994" max="9994" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="9995" max="9995" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="9996" max="9999" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10000" max="10000" width="6.7109375" style="4" customWidth="1"/>
-    <col min="10001" max="10002" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10003" max="10003" width="10.42578125" style="4" customWidth="1"/>
+    <col min="9996" max="9999" width="10.25" style="4" customWidth="1"/>
+    <col min="10000" max="10000" width="6.75" style="4" customWidth="1"/>
+    <col min="10001" max="10002" width="10.25" style="4" customWidth="1"/>
+    <col min="10003" max="10003" width="10.375" style="4" customWidth="1"/>
     <col min="10004" max="10007" width="9" style="4" customWidth="1"/>
-    <col min="10008" max="10008" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10009" max="10010" width="8.28515625" style="4" customWidth="1"/>
-    <col min="10011" max="10015" width="6.42578125" style="4" customWidth="1"/>
-    <col min="10016" max="10240" width="6.42578125" style="4"/>
+    <col min="10008" max="10008" width="10.25" style="4" customWidth="1"/>
+    <col min="10009" max="10010" width="8.25" style="4" customWidth="1"/>
+    <col min="10011" max="10015" width="6.375" style="4" customWidth="1"/>
+    <col min="10016" max="10240" width="6.375" style="4"/>
     <col min="10241" max="10241" width="2" style="4" customWidth="1"/>
-    <col min="10242" max="10242" width="7.5703125" style="4" customWidth="1"/>
+    <col min="10242" max="10242" width="7.625" style="4" customWidth="1"/>
     <col min="10243" max="10247" width="9" style="4" customWidth="1"/>
-    <col min="10248" max="10248" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10249" max="10249" width="12.7109375" style="4" customWidth="1"/>
+    <col min="10248" max="10248" width="10.25" style="4" customWidth="1"/>
+    <col min="10249" max="10249" width="12.75" style="4" customWidth="1"/>
     <col min="10250" max="10250" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="10251" max="10251" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="10252" max="10255" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10256" max="10256" width="6.7109375" style="4" customWidth="1"/>
-    <col min="10257" max="10258" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10259" max="10259" width="10.42578125" style="4" customWidth="1"/>
+    <col min="10252" max="10255" width="10.25" style="4" customWidth="1"/>
+    <col min="10256" max="10256" width="6.75" style="4" customWidth="1"/>
+    <col min="10257" max="10258" width="10.25" style="4" customWidth="1"/>
+    <col min="10259" max="10259" width="10.375" style="4" customWidth="1"/>
     <col min="10260" max="10263" width="9" style="4" customWidth="1"/>
-    <col min="10264" max="10264" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10265" max="10266" width="8.28515625" style="4" customWidth="1"/>
-    <col min="10267" max="10271" width="6.42578125" style="4" customWidth="1"/>
-    <col min="10272" max="10496" width="6.42578125" style="4"/>
+    <col min="10264" max="10264" width="10.25" style="4" customWidth="1"/>
+    <col min="10265" max="10266" width="8.25" style="4" customWidth="1"/>
+    <col min="10267" max="10271" width="6.375" style="4" customWidth="1"/>
+    <col min="10272" max="10496" width="6.375" style="4"/>
     <col min="10497" max="10497" width="2" style="4" customWidth="1"/>
-    <col min="10498" max="10498" width="7.5703125" style="4" customWidth="1"/>
+    <col min="10498" max="10498" width="7.625" style="4" customWidth="1"/>
     <col min="10499" max="10503" width="9" style="4" customWidth="1"/>
-    <col min="10504" max="10504" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10505" max="10505" width="12.7109375" style="4" customWidth="1"/>
+    <col min="10504" max="10504" width="10.25" style="4" customWidth="1"/>
+    <col min="10505" max="10505" width="12.75" style="4" customWidth="1"/>
     <col min="10506" max="10506" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="10507" max="10507" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="10508" max="10511" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10512" max="10512" width="6.7109375" style="4" customWidth="1"/>
-    <col min="10513" max="10514" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10515" max="10515" width="10.42578125" style="4" customWidth="1"/>
+    <col min="10508" max="10511" width="10.25" style="4" customWidth="1"/>
+    <col min="10512" max="10512" width="6.75" style="4" customWidth="1"/>
+    <col min="10513" max="10514" width="10.25" style="4" customWidth="1"/>
+    <col min="10515" max="10515" width="10.375" style="4" customWidth="1"/>
     <col min="10516" max="10519" width="9" style="4" customWidth="1"/>
-    <col min="10520" max="10520" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10521" max="10522" width="8.28515625" style="4" customWidth="1"/>
-    <col min="10523" max="10527" width="6.42578125" style="4" customWidth="1"/>
-    <col min="10528" max="10752" width="6.42578125" style="4"/>
+    <col min="10520" max="10520" width="10.25" style="4" customWidth="1"/>
+    <col min="10521" max="10522" width="8.25" style="4" customWidth="1"/>
+    <col min="10523" max="10527" width="6.375" style="4" customWidth="1"/>
+    <col min="10528" max="10752" width="6.375" style="4"/>
     <col min="10753" max="10753" width="2" style="4" customWidth="1"/>
-    <col min="10754" max="10754" width="7.5703125" style="4" customWidth="1"/>
+    <col min="10754" max="10754" width="7.625" style="4" customWidth="1"/>
     <col min="10755" max="10759" width="9" style="4" customWidth="1"/>
-    <col min="10760" max="10760" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10761" max="10761" width="12.7109375" style="4" customWidth="1"/>
+    <col min="10760" max="10760" width="10.25" style="4" customWidth="1"/>
+    <col min="10761" max="10761" width="12.75" style="4" customWidth="1"/>
     <col min="10762" max="10762" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="10763" max="10763" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="10764" max="10767" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10768" max="10768" width="6.7109375" style="4" customWidth="1"/>
-    <col min="10769" max="10770" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10771" max="10771" width="10.42578125" style="4" customWidth="1"/>
+    <col min="10764" max="10767" width="10.25" style="4" customWidth="1"/>
+    <col min="10768" max="10768" width="6.75" style="4" customWidth="1"/>
+    <col min="10769" max="10770" width="10.25" style="4" customWidth="1"/>
+    <col min="10771" max="10771" width="10.375" style="4" customWidth="1"/>
     <col min="10772" max="10775" width="9" style="4" customWidth="1"/>
-    <col min="10776" max="10776" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10777" max="10778" width="8.28515625" style="4" customWidth="1"/>
-    <col min="10779" max="10783" width="6.42578125" style="4" customWidth="1"/>
-    <col min="10784" max="11008" width="6.42578125" style="4"/>
+    <col min="10776" max="10776" width="10.25" style="4" customWidth="1"/>
+    <col min="10777" max="10778" width="8.25" style="4" customWidth="1"/>
+    <col min="10779" max="10783" width="6.375" style="4" customWidth="1"/>
+    <col min="10784" max="11008" width="6.375" style="4"/>
     <col min="11009" max="11009" width="2" style="4" customWidth="1"/>
-    <col min="11010" max="11010" width="7.5703125" style="4" customWidth="1"/>
+    <col min="11010" max="11010" width="7.625" style="4" customWidth="1"/>
     <col min="11011" max="11015" width="9" style="4" customWidth="1"/>
-    <col min="11016" max="11016" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11017" max="11017" width="12.7109375" style="4" customWidth="1"/>
+    <col min="11016" max="11016" width="10.25" style="4" customWidth="1"/>
+    <col min="11017" max="11017" width="12.75" style="4" customWidth="1"/>
     <col min="11018" max="11018" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="11019" max="11019" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="11020" max="11023" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11024" max="11024" width="6.7109375" style="4" customWidth="1"/>
-    <col min="11025" max="11026" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11027" max="11027" width="10.42578125" style="4" customWidth="1"/>
+    <col min="11020" max="11023" width="10.25" style="4" customWidth="1"/>
+    <col min="11024" max="11024" width="6.75" style="4" customWidth="1"/>
+    <col min="11025" max="11026" width="10.25" style="4" customWidth="1"/>
+    <col min="11027" max="11027" width="10.375" style="4" customWidth="1"/>
     <col min="11028" max="11031" width="9" style="4" customWidth="1"/>
-    <col min="11032" max="11032" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11033" max="11034" width="8.28515625" style="4" customWidth="1"/>
-    <col min="11035" max="11039" width="6.42578125" style="4" customWidth="1"/>
-    <col min="11040" max="11264" width="6.42578125" style="4"/>
+    <col min="11032" max="11032" width="10.25" style="4" customWidth="1"/>
+    <col min="11033" max="11034" width="8.25" style="4" customWidth="1"/>
+    <col min="11035" max="11039" width="6.375" style="4" customWidth="1"/>
+    <col min="11040" max="11264" width="6.375" style="4"/>
     <col min="11265" max="11265" width="2" style="4" customWidth="1"/>
-    <col min="11266" max="11266" width="7.5703125" style="4" customWidth="1"/>
+    <col min="11266" max="11266" width="7.625" style="4" customWidth="1"/>
     <col min="11267" max="11271" width="9" style="4" customWidth="1"/>
-    <col min="11272" max="11272" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11273" max="11273" width="12.7109375" style="4" customWidth="1"/>
+    <col min="11272" max="11272" width="10.25" style="4" customWidth="1"/>
+    <col min="11273" max="11273" width="12.75" style="4" customWidth="1"/>
     <col min="11274" max="11274" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="11275" max="11275" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="11276" max="11279" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11280" max="11280" width="6.7109375" style="4" customWidth="1"/>
-    <col min="11281" max="11282" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11283" max="11283" width="10.42578125" style="4" customWidth="1"/>
+    <col min="11276" max="11279" width="10.25" style="4" customWidth="1"/>
+    <col min="11280" max="11280" width="6.75" style="4" customWidth="1"/>
+    <col min="11281" max="11282" width="10.25" style="4" customWidth="1"/>
+    <col min="11283" max="11283" width="10.375" style="4" customWidth="1"/>
     <col min="11284" max="11287" width="9" style="4" customWidth="1"/>
-    <col min="11288" max="11288" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11289" max="11290" width="8.28515625" style="4" customWidth="1"/>
-    <col min="11291" max="11295" width="6.42578125" style="4" customWidth="1"/>
-    <col min="11296" max="11520" width="6.42578125" style="4"/>
+    <col min="11288" max="11288" width="10.25" style="4" customWidth="1"/>
+    <col min="11289" max="11290" width="8.25" style="4" customWidth="1"/>
+    <col min="11291" max="11295" width="6.375" style="4" customWidth="1"/>
+    <col min="11296" max="11520" width="6.375" style="4"/>
     <col min="11521" max="11521" width="2" style="4" customWidth="1"/>
-    <col min="11522" max="11522" width="7.5703125" style="4" customWidth="1"/>
+    <col min="11522" max="11522" width="7.625" style="4" customWidth="1"/>
     <col min="11523" max="11527" width="9" style="4" customWidth="1"/>
-    <col min="11528" max="11528" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11529" max="11529" width="12.7109375" style="4" customWidth="1"/>
+    <col min="11528" max="11528" width="10.25" style="4" customWidth="1"/>
+    <col min="11529" max="11529" width="12.75" style="4" customWidth="1"/>
     <col min="11530" max="11530" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="11531" max="11531" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="11532" max="11535" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11536" max="11536" width="6.7109375" style="4" customWidth="1"/>
-    <col min="11537" max="11538" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11539" max="11539" width="10.42578125" style="4" customWidth="1"/>
+    <col min="11532" max="11535" width="10.25" style="4" customWidth="1"/>
+    <col min="11536" max="11536" width="6.75" style="4" customWidth="1"/>
+    <col min="11537" max="11538" width="10.25" style="4" customWidth="1"/>
+    <col min="11539" max="11539" width="10.375" style="4" customWidth="1"/>
     <col min="11540" max="11543" width="9" style="4" customWidth="1"/>
-    <col min="11544" max="11544" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11545" max="11546" width="8.28515625" style="4" customWidth="1"/>
-    <col min="11547" max="11551" width="6.42578125" style="4" customWidth="1"/>
-    <col min="11552" max="11776" width="6.42578125" style="4"/>
+    <col min="11544" max="11544" width="10.25" style="4" customWidth="1"/>
+    <col min="11545" max="11546" width="8.25" style="4" customWidth="1"/>
+    <col min="11547" max="11551" width="6.375" style="4" customWidth="1"/>
+    <col min="11552" max="11776" width="6.375" style="4"/>
     <col min="11777" max="11777" width="2" style="4" customWidth="1"/>
-    <col min="11778" max="11778" width="7.5703125" style="4" customWidth="1"/>
+    <col min="11778" max="11778" width="7.625" style="4" customWidth="1"/>
     <col min="11779" max="11783" width="9" style="4" customWidth="1"/>
-    <col min="11784" max="11784" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11785" max="11785" width="12.7109375" style="4" customWidth="1"/>
+    <col min="11784" max="11784" width="10.25" style="4" customWidth="1"/>
+    <col min="11785" max="11785" width="12.75" style="4" customWidth="1"/>
     <col min="11786" max="11786" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="11787" max="11787" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="11788" max="11791" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11792" max="11792" width="6.7109375" style="4" customWidth="1"/>
-    <col min="11793" max="11794" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11795" max="11795" width="10.42578125" style="4" customWidth="1"/>
+    <col min="11788" max="11791" width="10.25" style="4" customWidth="1"/>
+    <col min="11792" max="11792" width="6.75" style="4" customWidth="1"/>
+    <col min="11793" max="11794" width="10.25" style="4" customWidth="1"/>
+    <col min="11795" max="11795" width="10.375" style="4" customWidth="1"/>
     <col min="11796" max="11799" width="9" style="4" customWidth="1"/>
-    <col min="11800" max="11800" width="10.28515625" style="4" customWidth="1"/>
-    <col min="11801" max="11802" width="8.28515625" style="4" customWidth="1"/>
-    <col min="11803" max="11807" width="6.42578125" style="4" customWidth="1"/>
-    <col min="11808" max="12032" width="6.42578125" style="4"/>
+    <col min="11800" max="11800" width="10.25" style="4" customWidth="1"/>
+    <col min="11801" max="11802" width="8.25" style="4" customWidth="1"/>
+    <col min="11803" max="11807" width="6.375" style="4" customWidth="1"/>
+    <col min="11808" max="12032" width="6.375" style="4"/>
     <col min="12033" max="12033" width="2" style="4" customWidth="1"/>
-    <col min="12034" max="12034" width="7.5703125" style="4" customWidth="1"/>
+    <col min="12034" max="12034" width="7.625" style="4" customWidth="1"/>
     <col min="12035" max="12039" width="9" style="4" customWidth="1"/>
-    <col min="12040" max="12040" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12041" max="12041" width="12.7109375" style="4" customWidth="1"/>
+    <col min="12040" max="12040" width="10.25" style="4" customWidth="1"/>
+    <col min="12041" max="12041" width="12.75" style="4" customWidth="1"/>
     <col min="12042" max="12042" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="12043" max="12043" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="12044" max="12047" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12048" max="12048" width="6.7109375" style="4" customWidth="1"/>
-    <col min="12049" max="12050" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12051" max="12051" width="10.42578125" style="4" customWidth="1"/>
+    <col min="12044" max="12047" width="10.25" style="4" customWidth="1"/>
+    <col min="12048" max="12048" width="6.75" style="4" customWidth="1"/>
+    <col min="12049" max="12050" width="10.25" style="4" customWidth="1"/>
+    <col min="12051" max="12051" width="10.375" style="4" customWidth="1"/>
     <col min="12052" max="12055" width="9" style="4" customWidth="1"/>
-    <col min="12056" max="12056" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12057" max="12058" width="8.28515625" style="4" customWidth="1"/>
-    <col min="12059" max="12063" width="6.42578125" style="4" customWidth="1"/>
-    <col min="12064" max="12288" width="6.42578125" style="4"/>
+    <col min="12056" max="12056" width="10.25" style="4" customWidth="1"/>
+    <col min="12057" max="12058" width="8.25" style="4" customWidth="1"/>
+    <col min="12059" max="12063" width="6.375" style="4" customWidth="1"/>
+    <col min="12064" max="12288" width="6.375" style="4"/>
     <col min="12289" max="12289" width="2" style="4" customWidth="1"/>
-    <col min="12290" max="12290" width="7.5703125" style="4" customWidth="1"/>
+    <col min="12290" max="12290" width="7.625" style="4" customWidth="1"/>
     <col min="12291" max="12295" width="9" style="4" customWidth="1"/>
-    <col min="12296" max="12296" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12297" max="12297" width="12.7109375" style="4" customWidth="1"/>
+    <col min="12296" max="12296" width="10.25" style="4" customWidth="1"/>
+    <col min="12297" max="12297" width="12.75" style="4" customWidth="1"/>
     <col min="12298" max="12298" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="12299" max="12299" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="12300" max="12303" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12304" max="12304" width="6.7109375" style="4" customWidth="1"/>
-    <col min="12305" max="12306" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12307" max="12307" width="10.42578125" style="4" customWidth="1"/>
+    <col min="12300" max="12303" width="10.25" style="4" customWidth="1"/>
+    <col min="12304" max="12304" width="6.75" style="4" customWidth="1"/>
+    <col min="12305" max="12306" width="10.25" style="4" customWidth="1"/>
+    <col min="12307" max="12307" width="10.375" style="4" customWidth="1"/>
     <col min="12308" max="12311" width="9" style="4" customWidth="1"/>
-    <col min="12312" max="12312" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12313" max="12314" width="8.28515625" style="4" customWidth="1"/>
-    <col min="12315" max="12319" width="6.42578125" style="4" customWidth="1"/>
-    <col min="12320" max="12544" width="6.42578125" style="4"/>
+    <col min="12312" max="12312" width="10.25" style="4" customWidth="1"/>
+    <col min="12313" max="12314" width="8.25" style="4" customWidth="1"/>
+    <col min="12315" max="12319" width="6.375" style="4" customWidth="1"/>
+    <col min="12320" max="12544" width="6.375" style="4"/>
     <col min="12545" max="12545" width="2" style="4" customWidth="1"/>
-    <col min="12546" max="12546" width="7.5703125" style="4" customWidth="1"/>
+    <col min="12546" max="12546" width="7.625" style="4" customWidth="1"/>
     <col min="12547" max="12551" width="9" style="4" customWidth="1"/>
-    <col min="12552" max="12552" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12553" max="12553" width="12.7109375" style="4" customWidth="1"/>
+    <col min="12552" max="12552" width="10.25" style="4" customWidth="1"/>
+    <col min="12553" max="12553" width="12.75" style="4" customWidth="1"/>
     <col min="12554" max="12554" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="12555" max="12555" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="12556" max="12559" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12560" max="12560" width="6.7109375" style="4" customWidth="1"/>
-    <col min="12561" max="12562" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12563" max="12563" width="10.42578125" style="4" customWidth="1"/>
+    <col min="12556" max="12559" width="10.25" style="4" customWidth="1"/>
+    <col min="12560" max="12560" width="6.75" style="4" customWidth="1"/>
+    <col min="12561" max="12562" width="10.25" style="4" customWidth="1"/>
+    <col min="12563" max="12563" width="10.375" style="4" customWidth="1"/>
     <col min="12564" max="12567" width="9" style="4" customWidth="1"/>
-    <col min="12568" max="12568" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12569" max="12570" width="8.28515625" style="4" customWidth="1"/>
-    <col min="12571" max="12575" width="6.42578125" style="4" customWidth="1"/>
-    <col min="12576" max="12800" width="6.42578125" style="4"/>
+    <col min="12568" max="12568" width="10.25" style="4" customWidth="1"/>
+    <col min="12569" max="12570" width="8.25" style="4" customWidth="1"/>
+    <col min="12571" max="12575" width="6.375" style="4" customWidth="1"/>
+    <col min="12576" max="12800" width="6.375" style="4"/>
     <col min="12801" max="12801" width="2" style="4" customWidth="1"/>
-    <col min="12802" max="12802" width="7.5703125" style="4" customWidth="1"/>
+    <col min="12802" max="12802" width="7.625" style="4" customWidth="1"/>
     <col min="12803" max="12807" width="9" style="4" customWidth="1"/>
-    <col min="12808" max="12808" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12809" max="12809" width="12.7109375" style="4" customWidth="1"/>
+    <col min="12808" max="12808" width="10.25" style="4" customWidth="1"/>
+    <col min="12809" max="12809" width="12.75" style="4" customWidth="1"/>
     <col min="12810" max="12810" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="12811" max="12811" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="12812" max="12815" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12816" max="12816" width="6.7109375" style="4" customWidth="1"/>
-    <col min="12817" max="12818" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12819" max="12819" width="10.42578125" style="4" customWidth="1"/>
+    <col min="12812" max="12815" width="10.25" style="4" customWidth="1"/>
+    <col min="12816" max="12816" width="6.75" style="4" customWidth="1"/>
+    <col min="12817" max="12818" width="10.25" style="4" customWidth="1"/>
+    <col min="12819" max="12819" width="10.375" style="4" customWidth="1"/>
     <col min="12820" max="12823" width="9" style="4" customWidth="1"/>
-    <col min="12824" max="12824" width="10.28515625" style="4" customWidth="1"/>
-    <col min="12825" max="12826" width="8.28515625" style="4" customWidth="1"/>
-    <col min="12827" max="12831" width="6.42578125" style="4" customWidth="1"/>
-    <col min="12832" max="13056" width="6.42578125" style="4"/>
+    <col min="12824" max="12824" width="10.25" style="4" customWidth="1"/>
+    <col min="12825" max="12826" width="8.25" style="4" customWidth="1"/>
+    <col min="12827" max="12831" width="6.375" style="4" customWidth="1"/>
+    <col min="12832" max="13056" width="6.375" style="4"/>
     <col min="13057" max="13057" width="2" style="4" customWidth="1"/>
-    <col min="13058" max="13058" width="7.5703125" style="4" customWidth="1"/>
+    <col min="13058" max="13058" width="7.625" style="4" customWidth="1"/>
     <col min="13059" max="13063" width="9" style="4" customWidth="1"/>
-    <col min="13064" max="13064" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13065" max="13065" width="12.7109375" style="4" customWidth="1"/>
+    <col min="13064" max="13064" width="10.25" style="4" customWidth="1"/>
+    <col min="13065" max="13065" width="12.75" style="4" customWidth="1"/>
     <col min="13066" max="13066" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="13067" max="13067" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="13068" max="13071" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13072" max="13072" width="6.7109375" style="4" customWidth="1"/>
-    <col min="13073" max="13074" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13075" max="13075" width="10.42578125" style="4" customWidth="1"/>
+    <col min="13068" max="13071" width="10.25" style="4" customWidth="1"/>
+    <col min="13072" max="13072" width="6.75" style="4" customWidth="1"/>
+    <col min="13073" max="13074" width="10.25" style="4" customWidth="1"/>
+    <col min="13075" max="13075" width="10.375" style="4" customWidth="1"/>
     <col min="13076" max="13079" width="9" style="4" customWidth="1"/>
-    <col min="13080" max="13080" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13081" max="13082" width="8.28515625" style="4" customWidth="1"/>
-    <col min="13083" max="13087" width="6.42578125" style="4" customWidth="1"/>
-    <col min="13088" max="13312" width="6.42578125" style="4"/>
+    <col min="13080" max="13080" width="10.25" style="4" customWidth="1"/>
+    <col min="13081" max="13082" width="8.25" style="4" customWidth="1"/>
+    <col min="13083" max="13087" width="6.375" style="4" customWidth="1"/>
+    <col min="13088" max="13312" width="6.375" style="4"/>
     <col min="13313" max="13313" width="2" style="4" customWidth="1"/>
-    <col min="13314" max="13314" width="7.5703125" style="4" customWidth="1"/>
+    <col min="13314" max="13314" width="7.625" style="4" customWidth="1"/>
     <col min="13315" max="13319" width="9" style="4" customWidth="1"/>
-    <col min="13320" max="13320" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13321" max="13321" width="12.7109375" style="4" customWidth="1"/>
+    <col min="13320" max="13320" width="10.25" style="4" customWidth="1"/>
+    <col min="13321" max="13321" width="12.75" style="4" customWidth="1"/>
     <col min="13322" max="13322" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="13323" max="13323" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="13324" max="13327" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13328" max="13328" width="6.7109375" style="4" customWidth="1"/>
-    <col min="13329" max="13330" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13331" max="13331" width="10.42578125" style="4" customWidth="1"/>
+    <col min="13324" max="13327" width="10.25" style="4" customWidth="1"/>
+    <col min="13328" max="13328" width="6.75" style="4" customWidth="1"/>
+    <col min="13329" max="13330" width="10.25" style="4" customWidth="1"/>
+    <col min="13331" max="13331" width="10.375" style="4" customWidth="1"/>
     <col min="13332" max="13335" width="9" style="4" customWidth="1"/>
-    <col min="13336" max="13336" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13337" max="13338" width="8.28515625" style="4" customWidth="1"/>
-    <col min="13339" max="13343" width="6.42578125" style="4" customWidth="1"/>
-    <col min="13344" max="13568" width="6.42578125" style="4"/>
+    <col min="13336" max="13336" width="10.25" style="4" customWidth="1"/>
+    <col min="13337" max="13338" width="8.25" style="4" customWidth="1"/>
+    <col min="13339" max="13343" width="6.375" style="4" customWidth="1"/>
+    <col min="13344" max="13568" width="6.375" style="4"/>
     <col min="13569" max="13569" width="2" style="4" customWidth="1"/>
-    <col min="13570" max="13570" width="7.5703125" style="4" customWidth="1"/>
+    <col min="13570" max="13570" width="7.625" style="4" customWidth="1"/>
     <col min="13571" max="13575" width="9" style="4" customWidth="1"/>
-    <col min="13576" max="13576" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13577" max="13577" width="12.7109375" style="4" customWidth="1"/>
+    <col min="13576" max="13576" width="10.25" style="4" customWidth="1"/>
+    <col min="13577" max="13577" width="12.75" style="4" customWidth="1"/>
     <col min="13578" max="13578" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="13579" max="13579" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="13580" max="13583" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13584" max="13584" width="6.7109375" style="4" customWidth="1"/>
-    <col min="13585" max="13586" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13587" max="13587" width="10.42578125" style="4" customWidth="1"/>
+    <col min="13580" max="13583" width="10.25" style="4" customWidth="1"/>
+    <col min="13584" max="13584" width="6.75" style="4" customWidth="1"/>
+    <col min="13585" max="13586" width="10.25" style="4" customWidth="1"/>
+    <col min="13587" max="13587" width="10.375" style="4" customWidth="1"/>
     <col min="13588" max="13591" width="9" style="4" customWidth="1"/>
-    <col min="13592" max="13592" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13593" max="13594" width="8.28515625" style="4" customWidth="1"/>
-    <col min="13595" max="13599" width="6.42578125" style="4" customWidth="1"/>
-    <col min="13600" max="13824" width="6.42578125" style="4"/>
+    <col min="13592" max="13592" width="10.25" style="4" customWidth="1"/>
+    <col min="13593" max="13594" width="8.25" style="4" customWidth="1"/>
+    <col min="13595" max="13599" width="6.375" style="4" customWidth="1"/>
+    <col min="13600" max="13824" width="6.375" style="4"/>
     <col min="13825" max="13825" width="2" style="4" customWidth="1"/>
-    <col min="13826" max="13826" width="7.5703125" style="4" customWidth="1"/>
+    <col min="13826" max="13826" width="7.625" style="4" customWidth="1"/>
     <col min="13827" max="13831" width="9" style="4" customWidth="1"/>
-    <col min="13832" max="13832" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13833" max="13833" width="12.7109375" style="4" customWidth="1"/>
+    <col min="13832" max="13832" width="10.25" style="4" customWidth="1"/>
+    <col min="13833" max="13833" width="12.75" style="4" customWidth="1"/>
     <col min="13834" max="13834" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="13835" max="13835" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="13836" max="13839" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13840" max="13840" width="6.7109375" style="4" customWidth="1"/>
-    <col min="13841" max="13842" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13843" max="13843" width="10.42578125" style="4" customWidth="1"/>
+    <col min="13836" max="13839" width="10.25" style="4" customWidth="1"/>
+    <col min="13840" max="13840" width="6.75" style="4" customWidth="1"/>
+    <col min="13841" max="13842" width="10.25" style="4" customWidth="1"/>
+    <col min="13843" max="13843" width="10.375" style="4" customWidth="1"/>
     <col min="13844" max="13847" width="9" style="4" customWidth="1"/>
-    <col min="13848" max="13848" width="10.28515625" style="4" customWidth="1"/>
-    <col min="13849" max="13850" width="8.28515625" style="4" customWidth="1"/>
-    <col min="13851" max="13855" width="6.42578125" style="4" customWidth="1"/>
-    <col min="13856" max="14080" width="6.42578125" style="4"/>
+    <col min="13848" max="13848" width="10.25" style="4" customWidth="1"/>
+    <col min="13849" max="13850" width="8.25" style="4" customWidth="1"/>
+    <col min="13851" max="13855" width="6.375" style="4" customWidth="1"/>
+    <col min="13856" max="14080" width="6.375" style="4"/>
     <col min="14081" max="14081" width="2" style="4" customWidth="1"/>
-    <col min="14082" max="14082" width="7.5703125" style="4" customWidth="1"/>
+    <col min="14082" max="14082" width="7.625" style="4" customWidth="1"/>
     <col min="14083" max="14087" width="9" style="4" customWidth="1"/>
-    <col min="14088" max="14088" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14089" max="14089" width="12.7109375" style="4" customWidth="1"/>
+    <col min="14088" max="14088" width="10.25" style="4" customWidth="1"/>
+    <col min="14089" max="14089" width="12.75" style="4" customWidth="1"/>
     <col min="14090" max="14090" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="14091" max="14091" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="14092" max="14095" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14096" max="14096" width="6.7109375" style="4" customWidth="1"/>
-    <col min="14097" max="14098" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14099" max="14099" width="10.42578125" style="4" customWidth="1"/>
+    <col min="14092" max="14095" width="10.25" style="4" customWidth="1"/>
+    <col min="14096" max="14096" width="6.75" style="4" customWidth="1"/>
+    <col min="14097" max="14098" width="10.25" style="4" customWidth="1"/>
+    <col min="14099" max="14099" width="10.375" style="4" customWidth="1"/>
     <col min="14100" max="14103" width="9" style="4" customWidth="1"/>
-    <col min="14104" max="14104" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14105" max="14106" width="8.28515625" style="4" customWidth="1"/>
-    <col min="14107" max="14111" width="6.42578125" style="4" customWidth="1"/>
-    <col min="14112" max="14336" width="6.42578125" style="4"/>
+    <col min="14104" max="14104" width="10.25" style="4" customWidth="1"/>
+    <col min="14105" max="14106" width="8.25" style="4" customWidth="1"/>
+    <col min="14107" max="14111" width="6.375" style="4" customWidth="1"/>
+    <col min="14112" max="14336" width="6.375" style="4"/>
     <col min="14337" max="14337" width="2" style="4" customWidth="1"/>
-    <col min="14338" max="14338" width="7.5703125" style="4" customWidth="1"/>
+    <col min="14338" max="14338" width="7.625" style="4" customWidth="1"/>
     <col min="14339" max="14343" width="9" style="4" customWidth="1"/>
-    <col min="14344" max="14344" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14345" max="14345" width="12.7109375" style="4" customWidth="1"/>
+    <col min="14344" max="14344" width="10.25" style="4" customWidth="1"/>
+    <col min="14345" max="14345" width="12.75" style="4" customWidth="1"/>
     <col min="14346" max="14346" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="14347" max="14347" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="14348" max="14351" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14352" max="14352" width="6.7109375" style="4" customWidth="1"/>
-    <col min="14353" max="14354" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14355" max="14355" width="10.42578125" style="4" customWidth="1"/>
+    <col min="14348" max="14351" width="10.25" style="4" customWidth="1"/>
+    <col min="14352" max="14352" width="6.75" style="4" customWidth="1"/>
+    <col min="14353" max="14354" width="10.25" style="4" customWidth="1"/>
+    <col min="14355" max="14355" width="10.375" style="4" customWidth="1"/>
     <col min="14356" max="14359" width="9" style="4" customWidth="1"/>
-    <col min="14360" max="14360" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14361" max="14362" width="8.28515625" style="4" customWidth="1"/>
-    <col min="14363" max="14367" width="6.42578125" style="4" customWidth="1"/>
-    <col min="14368" max="14592" width="6.42578125" style="4"/>
+    <col min="14360" max="14360" width="10.25" style="4" customWidth="1"/>
+    <col min="14361" max="14362" width="8.25" style="4" customWidth="1"/>
+    <col min="14363" max="14367" width="6.375" style="4" customWidth="1"/>
+    <col min="14368" max="14592" width="6.375" style="4"/>
     <col min="14593" max="14593" width="2" style="4" customWidth="1"/>
-    <col min="14594" max="14594" width="7.5703125" style="4" customWidth="1"/>
+    <col min="14594" max="14594" width="7.625" style="4" customWidth="1"/>
     <col min="14595" max="14599" width="9" style="4" customWidth="1"/>
-    <col min="14600" max="14600" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14601" max="14601" width="12.7109375" style="4" customWidth="1"/>
+    <col min="14600" max="14600" width="10.25" style="4" customWidth="1"/>
+    <col min="14601" max="14601" width="12.75" style="4" customWidth="1"/>
     <col min="14602" max="14602" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="14603" max="14603" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="14604" max="14607" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14608" max="14608" width="6.7109375" style="4" customWidth="1"/>
-    <col min="14609" max="14610" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14611" max="14611" width="10.42578125" style="4" customWidth="1"/>
+    <col min="14604" max="14607" width="10.25" style="4" customWidth="1"/>
+    <col min="14608" max="14608" width="6.75" style="4" customWidth="1"/>
+    <col min="14609" max="14610" width="10.25" style="4" customWidth="1"/>
+    <col min="14611" max="14611" width="10.375" style="4" customWidth="1"/>
     <col min="14612" max="14615" width="9" style="4" customWidth="1"/>
-    <col min="14616" max="14616" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14617" max="14618" width="8.28515625" style="4" customWidth="1"/>
-    <col min="14619" max="14623" width="6.42578125" style="4" customWidth="1"/>
-    <col min="14624" max="14848" width="6.42578125" style="4"/>
+    <col min="14616" max="14616" width="10.25" style="4" customWidth="1"/>
+    <col min="14617" max="14618" width="8.25" style="4" customWidth="1"/>
+    <col min="14619" max="14623" width="6.375" style="4" customWidth="1"/>
+    <col min="14624" max="14848" width="6.375" style="4"/>
     <col min="14849" max="14849" width="2" style="4" customWidth="1"/>
-    <col min="14850" max="14850" width="7.5703125" style="4" customWidth="1"/>
+    <col min="14850" max="14850" width="7.625" style="4" customWidth="1"/>
     <col min="14851" max="14855" width="9" style="4" customWidth="1"/>
-    <col min="14856" max="14856" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14857" max="14857" width="12.7109375" style="4" customWidth="1"/>
+    <col min="14856" max="14856" width="10.25" style="4" customWidth="1"/>
+    <col min="14857" max="14857" width="12.75" style="4" customWidth="1"/>
     <col min="14858" max="14858" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="14859" max="14859" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="14860" max="14863" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14864" max="14864" width="6.7109375" style="4" customWidth="1"/>
-    <col min="14865" max="14866" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14867" max="14867" width="10.42578125" style="4" customWidth="1"/>
+    <col min="14860" max="14863" width="10.25" style="4" customWidth="1"/>
+    <col min="14864" max="14864" width="6.75" style="4" customWidth="1"/>
+    <col min="14865" max="14866" width="10.25" style="4" customWidth="1"/>
+    <col min="14867" max="14867" width="10.375" style="4" customWidth="1"/>
     <col min="14868" max="14871" width="9" style="4" customWidth="1"/>
-    <col min="14872" max="14872" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14873" max="14874" width="8.28515625" style="4" customWidth="1"/>
-    <col min="14875" max="14879" width="6.42578125" style="4" customWidth="1"/>
-    <col min="14880" max="15104" width="6.42578125" style="4"/>
+    <col min="14872" max="14872" width="10.25" style="4" customWidth="1"/>
+    <col min="14873" max="14874" width="8.25" style="4" customWidth="1"/>
+    <col min="14875" max="14879" width="6.375" style="4" customWidth="1"/>
+    <col min="14880" max="15104" width="6.375" style="4"/>
     <col min="15105" max="15105" width="2" style="4" customWidth="1"/>
-    <col min="15106" max="15106" width="7.5703125" style="4" customWidth="1"/>
+    <col min="15106" max="15106" width="7.625" style="4" customWidth="1"/>
     <col min="15107" max="15111" width="9" style="4" customWidth="1"/>
-    <col min="15112" max="15112" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15113" max="15113" width="12.7109375" style="4" customWidth="1"/>
+    <col min="15112" max="15112" width="10.25" style="4" customWidth="1"/>
+    <col min="15113" max="15113" width="12.75" style="4" customWidth="1"/>
     <col min="15114" max="15114" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="15115" max="15115" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="15116" max="15119" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15120" max="15120" width="6.7109375" style="4" customWidth="1"/>
-    <col min="15121" max="15122" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15123" max="15123" width="10.42578125" style="4" customWidth="1"/>
+    <col min="15116" max="15119" width="10.25" style="4" customWidth="1"/>
+    <col min="15120" max="15120" width="6.75" style="4" customWidth="1"/>
+    <col min="15121" max="15122" width="10.25" style="4" customWidth="1"/>
+    <col min="15123" max="15123" width="10.375" style="4" customWidth="1"/>
     <col min="15124" max="15127" width="9" style="4" customWidth="1"/>
-    <col min="15128" max="15128" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15129" max="15130" width="8.28515625" style="4" customWidth="1"/>
-    <col min="15131" max="15135" width="6.42578125" style="4" customWidth="1"/>
-    <col min="15136" max="15360" width="6.42578125" style="4"/>
+    <col min="15128" max="15128" width="10.25" style="4" customWidth="1"/>
+    <col min="15129" max="15130" width="8.25" style="4" customWidth="1"/>
+    <col min="15131" max="15135" width="6.375" style="4" customWidth="1"/>
+    <col min="15136" max="15360" width="6.375" style="4"/>
     <col min="15361" max="15361" width="2" style="4" customWidth="1"/>
-    <col min="15362" max="15362" width="7.5703125" style="4" customWidth="1"/>
+    <col min="15362" max="15362" width="7.625" style="4" customWidth="1"/>
     <col min="15363" max="15367" width="9" style="4" customWidth="1"/>
-    <col min="15368" max="15368" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15369" max="15369" width="12.7109375" style="4" customWidth="1"/>
+    <col min="15368" max="15368" width="10.25" style="4" customWidth="1"/>
+    <col min="15369" max="15369" width="12.75" style="4" customWidth="1"/>
     <col min="15370" max="15370" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="15371" max="15371" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="15372" max="15375" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15376" max="15376" width="6.7109375" style="4" customWidth="1"/>
-    <col min="15377" max="15378" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15379" max="15379" width="10.42578125" style="4" customWidth="1"/>
+    <col min="15372" max="15375" width="10.25" style="4" customWidth="1"/>
+    <col min="15376" max="15376" width="6.75" style="4" customWidth="1"/>
+    <col min="15377" max="15378" width="10.25" style="4" customWidth="1"/>
+    <col min="15379" max="15379" width="10.375" style="4" customWidth="1"/>
     <col min="15380" max="15383" width="9" style="4" customWidth="1"/>
-    <col min="15384" max="15384" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15385" max="15386" width="8.28515625" style="4" customWidth="1"/>
-    <col min="15387" max="15391" width="6.42578125" style="4" customWidth="1"/>
-    <col min="15392" max="15616" width="6.42578125" style="4"/>
+    <col min="15384" max="15384" width="10.25" style="4" customWidth="1"/>
+    <col min="15385" max="15386" width="8.25" style="4" customWidth="1"/>
+    <col min="15387" max="15391" width="6.375" style="4" customWidth="1"/>
+    <col min="15392" max="15616" width="6.375" style="4"/>
     <col min="15617" max="15617" width="2" style="4" customWidth="1"/>
-    <col min="15618" max="15618" width="7.5703125" style="4" customWidth="1"/>
+    <col min="15618" max="15618" width="7.625" style="4" customWidth="1"/>
     <col min="15619" max="15623" width="9" style="4" customWidth="1"/>
-    <col min="15624" max="15624" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15625" max="15625" width="12.7109375" style="4" customWidth="1"/>
+    <col min="15624" max="15624" width="10.25" style="4" customWidth="1"/>
+    <col min="15625" max="15625" width="12.75" style="4" customWidth="1"/>
     <col min="15626" max="15626" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="15627" max="15627" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="15628" max="15631" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15632" max="15632" width="6.7109375" style="4" customWidth="1"/>
-    <col min="15633" max="15634" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15635" max="15635" width="10.42578125" style="4" customWidth="1"/>
+    <col min="15628" max="15631" width="10.25" style="4" customWidth="1"/>
+    <col min="15632" max="15632" width="6.75" style="4" customWidth="1"/>
+    <col min="15633" max="15634" width="10.25" style="4" customWidth="1"/>
+    <col min="15635" max="15635" width="10.375" style="4" customWidth="1"/>
     <col min="15636" max="15639" width="9" style="4" customWidth="1"/>
-    <col min="15640" max="15640" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15641" max="15642" width="8.28515625" style="4" customWidth="1"/>
-    <col min="15643" max="15647" width="6.42578125" style="4" customWidth="1"/>
-    <col min="15648" max="15872" width="6.42578125" style="4"/>
+    <col min="15640" max="15640" width="10.25" style="4" customWidth="1"/>
+    <col min="15641" max="15642" width="8.25" style="4" customWidth="1"/>
+    <col min="15643" max="15647" width="6.375" style="4" customWidth="1"/>
+    <col min="15648" max="15872" width="6.375" style="4"/>
     <col min="15873" max="15873" width="2" style="4" customWidth="1"/>
-    <col min="15874" max="15874" width="7.5703125" style="4" customWidth="1"/>
+    <col min="15874" max="15874" width="7.625" style="4" customWidth="1"/>
     <col min="15875" max="15879" width="9" style="4" customWidth="1"/>
-    <col min="15880" max="15880" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15881" max="15881" width="12.7109375" style="4" customWidth="1"/>
+    <col min="15880" max="15880" width="10.25" style="4" customWidth="1"/>
+    <col min="15881" max="15881" width="12.75" style="4" customWidth="1"/>
     <col min="15882" max="15882" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="15883" max="15883" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="15884" max="15887" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15888" max="15888" width="6.7109375" style="4" customWidth="1"/>
-    <col min="15889" max="15890" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15891" max="15891" width="10.42578125" style="4" customWidth="1"/>
+    <col min="15884" max="15887" width="10.25" style="4" customWidth="1"/>
+    <col min="15888" max="15888" width="6.75" style="4" customWidth="1"/>
+    <col min="15889" max="15890" width="10.25" style="4" customWidth="1"/>
+    <col min="15891" max="15891" width="10.375" style="4" customWidth="1"/>
     <col min="15892" max="15895" width="9" style="4" customWidth="1"/>
-    <col min="15896" max="15896" width="10.28515625" style="4" customWidth="1"/>
-    <col min="15897" max="15898" width="8.28515625" style="4" customWidth="1"/>
-    <col min="15899" max="15903" width="6.42578125" style="4" customWidth="1"/>
-    <col min="15904" max="16128" width="6.42578125" style="4"/>
+    <col min="15896" max="15896" width="10.25" style="4" customWidth="1"/>
+    <col min="15897" max="15898" width="8.25" style="4" customWidth="1"/>
+    <col min="15899" max="15903" width="6.375" style="4" customWidth="1"/>
+    <col min="15904" max="16128" width="6.375" style="4"/>
     <col min="16129" max="16129" width="2" style="4" customWidth="1"/>
-    <col min="16130" max="16130" width="7.5703125" style="4" customWidth="1"/>
+    <col min="16130" max="16130" width="7.625" style="4" customWidth="1"/>
     <col min="16131" max="16135" width="9" style="4" customWidth="1"/>
-    <col min="16136" max="16136" width="10.28515625" style="4" customWidth="1"/>
-    <col min="16137" max="16137" width="12.7109375" style="4" customWidth="1"/>
+    <col min="16136" max="16136" width="10.25" style="4" customWidth="1"/>
+    <col min="16137" max="16137" width="12.75" style="4" customWidth="1"/>
     <col min="16138" max="16138" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="16139" max="16139" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="16140" max="16143" width="10.28515625" style="4" customWidth="1"/>
-    <col min="16144" max="16144" width="6.7109375" style="4" customWidth="1"/>
-    <col min="16145" max="16146" width="10.28515625" style="4" customWidth="1"/>
-    <col min="16147" max="16147" width="10.42578125" style="4" customWidth="1"/>
+    <col min="16140" max="16143" width="10.25" style="4" customWidth="1"/>
+    <col min="16144" max="16144" width="6.75" style="4" customWidth="1"/>
+    <col min="16145" max="16146" width="10.25" style="4" customWidth="1"/>
+    <col min="16147" max="16147" width="10.375" style="4" customWidth="1"/>
     <col min="16148" max="16151" width="9" style="4" customWidth="1"/>
-    <col min="16152" max="16152" width="10.28515625" style="4" customWidth="1"/>
-    <col min="16153" max="16154" width="8.28515625" style="4" customWidth="1"/>
-    <col min="16155" max="16159" width="6.42578125" style="4" customWidth="1"/>
-    <col min="16160" max="16384" width="6.42578125" style="4"/>
+    <col min="16152" max="16152" width="10.25" style="4" customWidth="1"/>
+    <col min="16153" max="16154" width="8.25" style="4" customWidth="1"/>
+    <col min="16155" max="16159" width="6.375" style="4" customWidth="1"/>
+    <col min="16160" max="16384" width="6.375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:26" s="2" customFormat="1" ht="19.5" customHeight="1">
@@ -3412,75 +3396,75 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="2:26" ht="13.5" customHeight="1">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40" t="s">
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="N3" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
-      <c r="R3" s="40"/>
-      <c r="S3" s="40" t="s">
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="2:26" ht="12" customHeight="1">
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="40"/>
-      <c r="W4" s="40"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
@@ -3492,10 +3476,10 @@
       <c r="C5" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
       <c r="H5" s="6" t="s">
         <v>54</v>
       </c>
@@ -3510,30 +3494,30 @@
         <v>51</v>
       </c>
       <c r="M5" s="7"/>
-      <c r="N5" s="42" t="s">
+      <c r="N5" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="42"/>
-      <c r="W5" s="42"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
     </row>
     <row r="6" spans="2:26" s="8" customFormat="1" ht="291" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
       <c r="H6" s="6" t="s">
         <v>54</v>
       </c>
@@ -3551,27 +3535,27 @@
       <c r="N6" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
     </row>
     <row r="7" spans="2:26" s="8" customFormat="1" ht="29.25" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="6" t="s">
         <v>57</v>
       </c>
@@ -3589,15 +3573,15 @@
       <c r="N7" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
     </row>
     <row r="8" spans="2:26" s="8" customFormat="1" ht="43.5" customHeight="1">
       <c r="B8" s="5" t="s">
@@ -3606,10 +3590,10 @@
       <c r="C8" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
       <c r="H8" s="6" t="s">
         <v>22</v>
       </c>
@@ -3627,15 +3611,15 @@
       <c r="N8" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
+      <c r="V8" s="40"/>
+      <c r="W8" s="40"/>
     </row>
     <row r="9" spans="2:26" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="B9" s="34" t="s">
@@ -3673,7 +3657,7 @@
       <c r="B10" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="42" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="43"/>
@@ -3695,7 +3679,7 @@
       <c r="P10" s="43"/>
       <c r="Q10" s="43"/>
       <c r="R10" s="43"/>
-      <c r="S10" s="44" t="s">
+      <c r="S10" s="42" t="s">
         <v>79</v>
       </c>
       <c r="T10" s="43"/>
@@ -3707,7 +3691,7 @@
       <c r="B11" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="42" t="s">
         <v>80</v>
       </c>
       <c r="D11" s="43"/>
@@ -3744,10 +3728,10 @@
       <c r="C12" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
       <c r="H12" s="6" t="s">
         <v>22</v>
       </c>
@@ -3767,31 +3751,31 @@
         <v>41810</v>
       </c>
       <c r="N12" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
+        <v>105</v>
+      </c>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="40"/>
+      <c r="W12" s="40"/>
     </row>
     <row r="13" spans="2:26" s="8" customFormat="1" ht="115.5" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
+        <v>83</v>
+      </c>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
@@ -3802,70 +3786,70 @@
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="T13" s="42"/>
-      <c r="U13" s="42"/>
-      <c r="V13" s="42"/>
-      <c r="W13" s="42"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
     </row>
     <row r="14" spans="2:26" s="8" customFormat="1" ht="70.5" customHeight="1" collapsed="1">
       <c r="B14" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
+        <v>85</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
       <c r="H14" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K14" s="7">
         <v>41813</v>
       </c>
       <c r="L14" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M14" s="37"/>
       <c r="N14" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
-      <c r="U14" s="42"/>
-      <c r="V14" s="42"/>
-      <c r="W14" s="42"/>
+        <v>86</v>
+      </c>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="40"/>
     </row>
     <row r="15" spans="2:26" s="8" customFormat="1" ht="68.25" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
+        <v>89</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6" t="s">
@@ -3875,114 +3859,120 @@
         <v>41813</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M15" s="7"/>
       <c r="N15" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="42"/>
-      <c r="V15" s="42"/>
-      <c r="W15" s="42"/>
-    </row>
-    <row r="16" spans="2:26" s="8" customFormat="1" ht="32.25" customHeight="1">
+        <v>90</v>
+      </c>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+    </row>
+    <row r="16" spans="2:26" s="8" customFormat="1" ht="66.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
+      <c r="C16" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6" t="s">
         <v>47</v>
       </c>
       <c r="K16" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L16" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="L16" s="37" t="s">
-        <v>97</v>
-      </c>
       <c r="M16" s="37"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
-      <c r="U16" s="42"/>
-      <c r="V16" s="42"/>
-      <c r="W16" s="42"/>
-    </row>
-    <row r="17" spans="2:23" s="8" customFormat="1" ht="69" customHeight="1">
+      <c r="N16" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="40"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="40"/>
+      <c r="W16" s="40"/>
+    </row>
+    <row r="17" spans="2:23" s="8" customFormat="1" ht="84.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="6"/>
+      <c r="C17" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6" t="s">
         <v>47</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="M17" s="7">
         <v>41820</v>
       </c>
       <c r="N17" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
+        <v>113</v>
+      </c>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
       <c r="S17" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="T17" s="42"/>
-      <c r="U17" s="42"/>
-      <c r="V17" s="42"/>
-      <c r="W17" s="42"/>
+        <v>103</v>
+      </c>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="40"/>
     </row>
     <row r="18" spans="2:23" s="8" customFormat="1" ht="117" customHeight="1">
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="6"/>
+        <v>101</v>
+      </c>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L18" s="7" t="s">
         <v>51</v>
@@ -3991,123 +3981,151 @@
         <v>41820</v>
       </c>
       <c r="N18" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
+        <v>104</v>
+      </c>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
       <c r="S18" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="T18" s="42"/>
-      <c r="U18" s="42"/>
-      <c r="V18" s="42"/>
-      <c r="W18" s="42"/>
-    </row>
-    <row r="19" spans="2:23" s="8" customFormat="1" ht="15" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+    </row>
+    <row r="19" spans="2:23" s="8" customFormat="1" ht="37.5" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="6"/>
+      <c r="C19" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
-      <c r="U19" s="42"/>
-      <c r="V19" s="42"/>
-      <c r="W19" s="42"/>
-    </row>
-    <row r="20" spans="2:23" s="8" customFormat="1" ht="15" customHeight="1">
+      <c r="J19" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K19" s="7">
+        <v>41821</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M19" s="7">
+        <v>41821</v>
+      </c>
+      <c r="N19" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="40"/>
+      <c r="W19" s="40"/>
+    </row>
+    <row r="20" spans="2:23" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="B20" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
-      <c r="S20" s="42"/>
-      <c r="T20" s="42"/>
-      <c r="U20" s="42"/>
-      <c r="V20" s="42"/>
-      <c r="W20" s="42"/>
+      <c r="J20" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K20" s="7">
+        <v>41821</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="M20" s="7">
+        <v>41821</v>
+      </c>
+      <c r="N20" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="40"/>
     </row>
     <row r="21" spans="2:23" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="B21" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
+        <v>99</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="7"/>
       <c r="L21" s="6"/>
       <c r="M21" s="7"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
-      <c r="S21" s="42"/>
-      <c r="T21" s="42"/>
-      <c r="U21" s="42"/>
-      <c r="V21" s="42"/>
-      <c r="W21" s="42"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="40"/>
+      <c r="W21" s="40"/>
     </row>
     <row r="22" spans="2:23" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="B22" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
+        <v>100</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="7"/>
       <c r="L22" s="6"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="42"/>
-      <c r="T22" s="42"/>
-      <c r="U22" s="42"/>
-      <c r="V22" s="42"/>
-      <c r="W22" s="42"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="40"/>
+      <c r="W22" s="40"/>
     </row>
     <row r="26" spans="2:23" ht="15" hidden="1" customHeight="1" thickBot="1">
       <c r="B26" s="9" t="s">
@@ -4266,60 +4284,6 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="N21:R21"/>
-    <mergeCell ref="S21:W21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="N22:R22"/>
-    <mergeCell ref="S22:W22"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="S17:W17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="N18:R18"/>
-    <mergeCell ref="S18:W18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="S19:W19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="N20:R20"/>
-    <mergeCell ref="S20:W20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="S15:W15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="S16:W16"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="N13:R13"/>
-    <mergeCell ref="S13:W13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="S14:W14"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="S11:W11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="N12:R12"/>
-    <mergeCell ref="S12:W12"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="N10:R10"/>
-    <mergeCell ref="S10:W10"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="S7:W7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="S8:W8"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="S5:W5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="S6:W6"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:G4"/>
@@ -4330,21 +4294,75 @@
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="N3:R4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="S5:W5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="S6:W6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="S7:W7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="S8:W8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="N10:R10"/>
+    <mergeCell ref="S10:W10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="S11:W11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="N12:R12"/>
+    <mergeCell ref="S12:W12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="N13:R13"/>
+    <mergeCell ref="S13:W13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="S14:W14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="N15:R15"/>
+    <mergeCell ref="S15:W15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="S16:W16"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="S19:W19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="N20:R20"/>
+    <mergeCell ref="S20:W20"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="S17:W17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="N18:R18"/>
+    <mergeCell ref="S18:W18"/>
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="S21:W21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="N22:R22"/>
+    <mergeCell ref="S22:W22"/>
+    <mergeCell ref="C21:G21"/>
   </mergeCells>
   <phoneticPr fontId="37" type="noConversion"/>
-  <conditionalFormatting sqref="H5:W13 H14:I15 K14:W15 B5:C22 H16:W22 L14:L18">
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="H5:W13 H14:I15 K14:W15 B5:C22 L14:L19 H16:W22">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>OR($I5=Stop,#REF!=AllFinish,#REF!=NoToDo)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
       <formula>OR($I5=Ans)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
       <formula>OR($I14=Stop,#REF!=AllFinish,#REF!=NoToDo)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
       <formula>OR($I14=Ans)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update doc @Author : Alex
</commit_message>
<xml_diff>
--- a/05 Q&A/问答一览表.xlsx
+++ b/05 Q&A/问答一览表.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="122">
   <si>
     <t>版本履历</t>
   </si>
@@ -485,6 +485,123 @@
     <t>开发</t>
     <phoneticPr fontId="37" type="noConversion"/>
   </si>
+  <si>
+    <t>开发</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载日志</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄国腾</t>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">一  获取下载地址URL日志（共计18个字段）：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="黑体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>dlIndex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="黑体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+userCode
+IMSI
+IMEI
+version
+preassemble
+clientVersion
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="黑体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>accessType  81</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="黑体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="黑体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>productIndex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="黑体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+positionClient（客户侧真实排序号）
+positionindex（服务器侧排序号)
+spID
+updated
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="黑体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>channel     (沃商店：0 沃游戏：00018589)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="黑体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+referer
+status
+server_time
+IP
+日志文件名： mobile_wap_getURL</t>
+    </r>
+    <phoneticPr fontId="37" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -494,7 +611,7 @@
     <numFmt numFmtId="176" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
     <numFmt numFmtId="177" formatCode="yy/mm/dd"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,6 +874,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="黑体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="28">
@@ -1390,20 +1514,20 @@
     <xf numFmtId="0" fontId="32" fillId="26" borderId="19" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="57">
@@ -1465,21 +1589,7 @@
     <cellStyle name="未定義" xfId="44"/>
     <cellStyle name="原価計算" xfId="39"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="53"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -2297,15 +2407,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F8:I8"/>
@@ -2318,6 +2419,15 @@
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
   </mergeCells>
   <phoneticPr fontId="37" type="noConversion"/>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.31458333333333299" footer="0.31458333333333299"/>
@@ -2337,10 +2447,10 @@
   <dimension ref="B1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="4" topLeftCell="L17" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="11" ySplit="4" topLeftCell="L19" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.375" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
@@ -3396,75 +3506,75 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="2:26" ht="13.5" customHeight="1">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="44" t="s">
+      <c r="N3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44" t="s">
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="2:26" ht="12" customHeight="1">
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="44"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
@@ -3476,10 +3586,10 @@
       <c r="C5" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="6" t="s">
         <v>54</v>
       </c>
@@ -3494,30 +3604,30 @@
         <v>51</v>
       </c>
       <c r="M5" s="7"/>
-      <c r="N5" s="40" t="s">
+      <c r="N5" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="40"/>
-      <c r="W5" s="40"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="42"/>
     </row>
     <row r="6" spans="2:26" s="8" customFormat="1" ht="291" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="6" t="s">
         <v>54</v>
       </c>
@@ -3535,27 +3645,27 @@
       <c r="N6" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
-      <c r="V6" s="40"/>
-      <c r="W6" s="40"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="42"/>
+      <c r="V6" s="42"/>
+      <c r="W6" s="42"/>
     </row>
     <row r="7" spans="2:26" s="8" customFormat="1" ht="29.25" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="6" t="s">
         <v>57</v>
       </c>
@@ -3573,15 +3683,15 @@
       <c r="N7" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="40"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="40"/>
-      <c r="W7" s="40"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="42"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="42"/>
     </row>
     <row r="8" spans="2:26" s="8" customFormat="1" ht="43.5" customHeight="1">
       <c r="B8" s="5" t="s">
@@ -3590,10 +3700,10 @@
       <c r="C8" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="6" t="s">
         <v>22</v>
       </c>
@@ -3611,15 +3721,15 @@
       <c r="N8" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="40"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="40"/>
-      <c r="W8" s="40"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="42"/>
+      <c r="V8" s="42"/>
+      <c r="W8" s="42"/>
     </row>
     <row r="9" spans="2:26" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="B9" s="34" t="s">
@@ -3657,7 +3767,7 @@
       <c r="B10" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="44" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="43"/>
@@ -3679,7 +3789,7 @@
       <c r="P10" s="43"/>
       <c r="Q10" s="43"/>
       <c r="R10" s="43"/>
-      <c r="S10" s="42" t="s">
+      <c r="S10" s="44" t="s">
         <v>79</v>
       </c>
       <c r="T10" s="43"/>
@@ -3691,7 +3801,7 @@
       <c r="B11" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="44" t="s">
         <v>80</v>
       </c>
       <c r="D11" s="43"/>
@@ -3728,10 +3838,10 @@
       <c r="C12" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="6" t="s">
         <v>22</v>
       </c>
@@ -3753,15 +3863,15 @@
       <c r="N12" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="40"/>
-      <c r="T12" s="40"/>
-      <c r="U12" s="40"/>
-      <c r="V12" s="40"/>
-      <c r="W12" s="40"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="42"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="42"/>
     </row>
     <row r="13" spans="2:26" s="8" customFormat="1" ht="115.5" customHeight="1">
       <c r="B13" s="5" t="s">
@@ -3770,10 +3880,10 @@
       <c r="C13" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="6" t="s">
         <v>92</v>
       </c>
@@ -3786,18 +3896,18 @@
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="40"/>
-      <c r="S13" s="40" t="s">
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="T13" s="40"/>
-      <c r="U13" s="40"/>
-      <c r="V13" s="40"/>
-      <c r="W13" s="40"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="42"/>
+      <c r="V13" s="42"/>
+      <c r="W13" s="42"/>
     </row>
     <row r="14" spans="2:26" s="8" customFormat="1" ht="70.5" customHeight="1" collapsed="1">
       <c r="B14" s="5" t="s">
@@ -3806,10 +3916,10 @@
       <c r="C14" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="6" t="s">
         <v>93</v>
       </c>
@@ -3827,15 +3937,15 @@
       <c r="N14" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="40"/>
-      <c r="T14" s="40"/>
-      <c r="U14" s="40"/>
-      <c r="V14" s="40"/>
-      <c r="W14" s="40"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="42"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="42"/>
     </row>
     <row r="15" spans="2:26" s="8" customFormat="1" ht="68.25" customHeight="1">
       <c r="B15" s="5" t="s">
@@ -3844,10 +3954,10 @@
       <c r="C15" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
       <c r="H15" s="6" t="s">
         <v>92</v>
       </c>
@@ -3865,27 +3975,27 @@
       <c r="N15" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40"/>
-      <c r="S15" s="40"/>
-      <c r="T15" s="40"/>
-      <c r="U15" s="40"/>
-      <c r="V15" s="40"/>
-      <c r="W15" s="40"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="42"/>
     </row>
     <row r="16" spans="2:26" s="8" customFormat="1" ht="66.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6" t="s">
@@ -3901,27 +4011,27 @@
       <c r="N16" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="40"/>
-      <c r="S16" s="40"/>
-      <c r="T16" s="40"/>
-      <c r="U16" s="40"/>
-      <c r="V16" s="40"/>
-      <c r="W16" s="40"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42"/>
+      <c r="V16" s="42"/>
+      <c r="W16" s="42"/>
     </row>
     <row r="17" spans="2:23" s="8" customFormat="1" ht="84.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="6" t="s">
         <v>110</v>
       </c>
@@ -3941,17 +4051,17 @@
       <c r="N17" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="40"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="42"/>
       <c r="S17" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="T17" s="40"/>
-      <c r="U17" s="40"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="40"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="42"/>
+      <c r="V17" s="42"/>
+      <c r="W17" s="42"/>
     </row>
     <row r="18" spans="2:23" s="8" customFormat="1" ht="117" customHeight="1">
       <c r="B18" s="5" t="s">
@@ -3960,10 +4070,10 @@
       <c r="C18" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="6" t="s">
         <v>110</v>
       </c>
@@ -3983,17 +4093,17 @@
       <c r="N18" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="40"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
       <c r="S18" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="T18" s="40"/>
-      <c r="U18" s="40"/>
-      <c r="V18" s="40"/>
-      <c r="W18" s="40"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="V18" s="42"/>
+      <c r="W18" s="42"/>
     </row>
     <row r="19" spans="2:23" s="8" customFormat="1" ht="37.5" customHeight="1">
       <c r="B19" s="5" t="s">
@@ -4002,10 +4112,10 @@
       <c r="C19" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="6" t="s">
         <v>92</v>
       </c>
@@ -4025,27 +4135,27 @@
       <c r="N19" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="40"/>
-      <c r="T19" s="40"/>
-      <c r="U19" s="40"/>
-      <c r="V19" s="40"/>
-      <c r="W19" s="40"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="42"/>
     </row>
     <row r="20" spans="2:23" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="6" t="s">
         <v>117</v>
       </c>
@@ -4065,67 +4175,81 @@
       <c r="N20" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="40"/>
-      <c r="S20" s="40"/>
-      <c r="T20" s="40"/>
-      <c r="U20" s="40"/>
-      <c r="V20" s="40"/>
-      <c r="W20" s="40"/>
-    </row>
-    <row r="21" spans="2:23" s="8" customFormat="1" ht="15" customHeight="1">
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="42"/>
+      <c r="V20" s="42"/>
+      <c r="W20" s="42"/>
+    </row>
+    <row r="21" spans="2:23" s="8" customFormat="1" ht="254.25" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="6"/>
+      <c r="C21" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="6" t="s">
+        <v>118</v>
+      </c>
       <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="40"/>
-      <c r="S21" s="40"/>
-      <c r="T21" s="40"/>
-      <c r="U21" s="40"/>
-      <c r="V21" s="40"/>
-      <c r="W21" s="40"/>
+      <c r="J21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K21" s="7">
+        <v>41829</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M21" s="7">
+        <v>41829</v>
+      </c>
+      <c r="N21" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="42"/>
+      <c r="U21" s="42"/>
+      <c r="V21" s="42"/>
+      <c r="W21" s="42"/>
     </row>
     <row r="22" spans="2:23" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="B22" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="7"/>
       <c r="L22" s="6"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
-      <c r="S22" s="40"/>
-      <c r="T22" s="40"/>
-      <c r="U22" s="40"/>
-      <c r="V22" s="40"/>
-      <c r="W22" s="40"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="42"/>
+      <c r="W22" s="42"/>
     </row>
     <row r="26" spans="2:23" ht="15" hidden="1" customHeight="1" thickBot="1">
       <c r="B26" s="9" t="s">
@@ -4284,6 +4408,60 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="S21:W21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="N22:R22"/>
+    <mergeCell ref="S22:W22"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="S17:W17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="N18:R18"/>
+    <mergeCell ref="S18:W18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="S19:W19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="N20:R20"/>
+    <mergeCell ref="S20:W20"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="N15:R15"/>
+    <mergeCell ref="S15:W15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="S16:W16"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="N13:R13"/>
+    <mergeCell ref="S13:W13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="S14:W14"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="S11:W11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="N12:R12"/>
+    <mergeCell ref="S12:W12"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="N10:R10"/>
+    <mergeCell ref="S10:W10"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="S7:W7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="S8:W8"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="S5:W5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="S6:W6"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:G4"/>
@@ -4294,75 +4472,21 @@
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="N3:R4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="S5:W5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="S6:W6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="S7:W7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="S8:W8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="N10:R10"/>
-    <mergeCell ref="S10:W10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="S11:W11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="N12:R12"/>
-    <mergeCell ref="S12:W12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="N13:R13"/>
-    <mergeCell ref="S13:W13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="S14:W14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="S15:W15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="S16:W16"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="S19:W19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="N20:R20"/>
-    <mergeCell ref="S20:W20"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="S17:W17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="N18:R18"/>
-    <mergeCell ref="S18:W18"/>
-    <mergeCell ref="N21:R21"/>
-    <mergeCell ref="S21:W21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="N22:R22"/>
-    <mergeCell ref="S22:W22"/>
-    <mergeCell ref="C21:G21"/>
   </mergeCells>
   <phoneticPr fontId="37" type="noConversion"/>
   <conditionalFormatting sqref="H5:W13 H14:I15 K14:W15 B5:C22 L14:L19 H16:W22">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>OR($I5=Stop,#REF!=AllFinish,#REF!=NoToDo)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>OR($I5=Ans)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
       <formula>OR($I14=Stop,#REF!=AllFinish,#REF!=NoToDo)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="10" stopIfTrue="1">
       <formula>OR($I14=Ans)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>